<commit_message>
changed redirect to homepage
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTAutomatedTesting\seleniumTestingFramework\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04BCC9C-8CB6-444F-B336-6038C19B44F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0207996-FF6C-4974-9A73-E5B46D1CAF2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
   <si>
     <t>Sujith</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>JE Lease 111</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -2055,8 +2061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81362EF-F639-4F16-9B39-A84C1506E605}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,6 +2196,9 @@
       <c r="R2" t="b">
         <v>1</v>
       </c>
+      <c r="S2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2239,6 +2248,9 @@
       </c>
       <c r="R3" t="b">
         <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2485,7 +2497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD612C6E-0C35-4A08-BC9E-BAB6CEE21F73}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add: Add Recurrent Payment. Remove: SpaceCreate.java
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -5,25 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTAutomatedTesting\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CC828A-12EA-4484-905A-765AB73F5A10}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3204DF0-6A55-41A5-9398-917B27B29539}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
-    <sheet name="Property" sheetId="2" r:id="rId2"/>
-    <sheet name="Lease" sheetId="3" r:id="rId3"/>
-    <sheet name="Space" sheetId="4" r:id="rId4"/>
+    <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId2"/>
+    <sheet name="Property" sheetId="2" r:id="rId3"/>
+    <sheet name="Lease" sheetId="3" r:id="rId4"/>
+    <sheet name="Space" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>Sujith</t>
   </si>
@@ -136,9 +137,6 @@
     <t>contractTerm</t>
   </si>
   <si>
-    <t>JE Lease 111</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
@@ -149,9 +147,6 @@
   </si>
   <si>
     <t>01/01/2017</t>
-  </si>
-  <si>
-    <t>12/31/2019</t>
   </si>
   <si>
     <t>LeaseName</t>
@@ -193,32 +188,71 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>P_Test_Property_03</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
-    <t>Q_Test_Property</t>
+    <t>FASB - Charge</t>
   </si>
   <si>
-    <t>jjjj</t>
+    <t>Monthly</t>
   </si>
   <si>
-    <t>P_Test_Property_09</t>
+    <t>No Increase</t>
   </si>
   <si>
-    <t>P_Test_Property_01_Lease_Space_09</t>
+    <t>1st of Month After</t>
+  </si>
+  <si>
+    <t>Calendar Year</t>
+  </si>
+  <si>
+    <t>1250</t>
+  </si>
+  <si>
+    <t>chargeType</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>escalationType</t>
+  </si>
+  <si>
+    <t>leaseTermYear</t>
+  </si>
+  <si>
+    <t>leaseTermDefined</t>
+  </si>
+  <si>
+    <t>effDate</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Lease</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Lease_01</t>
+  </si>
+  <si>
+    <t>12/31/2021</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Lease_space_01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -229,6 +263,21 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -245,7 +294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -279,11 +328,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -319,6 +383,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,6 +724,1113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF54C438-284B-408F-94AA-81616ADED1B1}">
+  <dimension ref="A1:Z1000"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="20" style="12" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="12" customWidth="1"/>
+    <col min="8" max="9" width="21.28515625" style="12" customWidth="1"/>
+    <col min="10" max="11" width="14.42578125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="12" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" style="12" customWidth="1"/>
+    <col min="14" max="26" width="8.7109375" style="12" customWidth="1"/>
+    <col min="27" max="16384" width="14.42578125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B3" s="13"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
@@ -1994,11 +3192,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2096,107 +3294,69 @@
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>61</v>
+      <c r="D2" s="23" t="s">
+        <v>69</v>
       </c>
       <c r="E2" s="11">
-        <v>331112222</v>
+        <v>124564125</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="I2">
         <v>1229</v>
       </c>
       <c r="J2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="N2">
+        <v>100000000</v>
+      </c>
+      <c r="O2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="N2">
-        <v>12</v>
-      </c>
-      <c r="O2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3">
-        <v>1229</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3">
-        <v>12</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="R3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S3" t="s">
-        <v>57</v>
-      </c>
+      <c r="A3" s="6"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
@@ -5195,12 +6355,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5210,7 +6370,7 @@
     <col min="3" max="3" width="29.140625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" customWidth="1"/>
@@ -5219,7 +6379,7 @@
     <col min="13" max="13" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -5264,39 +6424,37 @@
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
-      <c r="D2" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>42</v>
+      <c r="K2" s="26" t="s">
+        <v>72</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>60</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
@@ -9390,11 +10548,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -9421,13 +10579,13 @@
         <v>11</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>27</v>
@@ -9457,17 +10615,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="13"/>
-      <c r="D2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>62</v>
+      <c r="D2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
handle critical step; run prerequisite before testcases
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C540373-E0C5-4102-87D0-C201F0352132}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B52DB0-9727-47B0-AB3F-97E9D2DD3FF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>ExecutionFlag</t>
-  </si>
-  <si>
-    <t>001</t>
   </si>
   <si>
     <t>dbaName</t>
@@ -217,32 +214,23 @@
     <t>Test_Property_Lease_01</t>
   </si>
   <si>
-    <t>STestProperty</t>
-  </si>
-  <si>
     <t>spaceInfo</t>
   </si>
   <si>
     <t>1251</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Test_Property_Auto_10_Lease_Space_30</t>
   </si>
   <si>
-    <t>JE Lease 555</t>
-  </si>
-  <si>
-    <t>W_Test_Property_10_Lease_Space_20</t>
-  </si>
-  <si>
-    <t>W_Test_Property_10_Lease_Space_21</t>
+    <t>Test_Property_Auto_10_Lease_Space_31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -268,18 +256,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -343,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -400,13 +376,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -725,7 +696,7 @@
   <dimension ref="A1:AA998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -748,7 +719,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -757,34 +728,34 @@
         <v>1</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="18" t="s">
         <v>57</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>58</v>
       </c>
       <c r="N1" s="11" t="s">
         <v>17</v>
@@ -809,77 +780,77 @@
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="14"/>
-      <c r="D2" s="27" t="s">
-        <v>68</v>
+      <c r="D2" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="J2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>50</v>
-      </c>
       <c r="N2" s="16" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="D3" s="27" t="s">
-        <v>68</v>
+      <c r="D3" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="J3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="K3" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1872,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1902,7 +1873,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1967,56 +1938,56 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>18</v>
+      <c r="A2" s="14">
+        <v>1</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="5">
         <v>124564125</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2">
+        <v>12229</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I2">
-        <v>1229</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="N2">
         <v>100000000</v>
       </c>
       <c r="O2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -5035,8 +5006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5058,7 +5029,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -5070,66 +5041,68 @@
         <v>2</v>
       </c>
       <c r="E1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="K1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="18" t="s">
         <v>25</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>26</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="25" t="s">
-        <v>64</v>
+      <c r="D2" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="I2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="J2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="19" t="s">
-        <v>30</v>
-      </c>
       <c r="K2" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N2" s="19"/>
     </row>
@@ -5140,9 +5113,9 @@
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
@@ -5155,9 +5128,9 @@
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
@@ -5170,9 +5143,9 @@
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
@@ -5185,9 +5158,9 @@
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
@@ -5200,9 +5173,9 @@
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
@@ -5214,9 +5187,9 @@
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
@@ -5228,9 +5201,9 @@
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
@@ -5242,9 +5215,9 @@
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
@@ -5256,9 +5229,9 @@
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
@@ -9247,7 +9220,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -9256,13 +9229,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>17</v>
@@ -9292,17 +9265,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="D2" s="27" t="s">
-        <v>68</v>
+      <c r="D2" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -9310,17 +9283,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="D3" s="27" t="s">
-        <v>68</v>
+      <c r="D3" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F3" s="6">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10305,6 +10278,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
search list of lease and space;property delete;refactor LeaseCreate file
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10B96A3-BD17-4DCF-AEA1-B1A5C17F28D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478A757D-9663-4D02-8C78-D0C63C0C677C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="96">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -224,6 +224,93 @@
   </si>
   <si>
     <t>Simon</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Final-04</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto-04</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Final_10_Lease_Space_31</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Final_10_Lease_Space_32</t>
+  </si>
+  <si>
+    <t>666677778</t>
+  </si>
+  <si>
+    <t>666677779</t>
+  </si>
+  <si>
+    <t>666677780</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto-01</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Final-02</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto-02</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Final-03</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto-03</t>
+  </si>
+  <si>
+    <t>1251</t>
+  </si>
+  <si>
+    <t>1252</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Final_10_Lease_Space_33</t>
+  </si>
+  <si>
+    <t>1253</t>
+  </si>
+  <si>
+    <t>BRT - Base Rent Retail</t>
+  </si>
+  <si>
+    <t>BRS - Base Rent Storage</t>
+  </si>
+  <si>
+    <t>BRO - Base Rent Office</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Final_10_Lease_Space_34</t>
+  </si>
+  <si>
+    <t>1254</t>
+  </si>
+  <si>
+    <t>666677774</t>
+  </si>
+  <si>
+    <t>Add2</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto</t>
+  </si>
+  <si>
+    <t>666677781</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto-07</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Final-07</t>
+  </si>
+  <si>
+    <t>Test_Property_Auto_Final_10_Lease_Space_37</t>
   </si>
 </sst>
 </file>
@@ -696,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF54C438-284B-408F-94AA-81616ADED1B1}">
   <dimension ref="A1:AA997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -810,6 +897,162 @@
         <v>39</v>
       </c>
       <c r="N2" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="D3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="D4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="D5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="D6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="N6" s="11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1803,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1812,7 +2055,7 @@
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
@@ -1947,11 +2190,61 @@
         <v>1</v>
       </c>
       <c r="S2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3">
+        <v>12230</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3">
+        <v>100000000</v>
+      </c>
+      <c r="O3">
+        <v>1000</v>
+      </c>
+      <c r="P3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -4952,10 +5245,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P1000"/>
+  <dimension ref="A1:P997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5039,10 +5332,10 @@
         <v>666677773</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>22</v>
@@ -5063,7 +5356,7 @@
         <v>66</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="O2" s="14" t="s">
         <v>58</v>
@@ -5073,40 +5366,180 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="A3" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="20">
+        <v>666677773</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="A4" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="20">
+        <v>666677773</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="A5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="20">
+        <v>666677773</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
+      <c r="A6" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="20">
+        <v>666677774</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
@@ -5128,30 +5561,15 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
@@ -5177,15 +5595,15 @@
       <c r="A17" s="12"/>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="G20" s="12"/>
     </row>
@@ -9096,18 +9514,6 @@
     <row r="997" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A997" s="12"/>
       <c r="G997" s="12"/>
-    </row>
-    <row r="998" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A998" s="12"/>
-      <c r="G998" s="12"/>
-    </row>
-    <row r="999" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A999" s="12"/>
-      <c r="G999" s="12"/>
-    </row>
-    <row r="1000" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1000" s="12"/>
-      <c r="G1000" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -9120,7 +9526,7 @@
   <dimension ref="A1:AB999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9130,7 +9536,7 @@
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="29.5703125" style="11" customWidth="1"/>
     <col min="6" max="6" width="31.85546875" customWidth="1"/>
-    <col min="7" max="7" width="40.28515625" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="28" width="8.7109375" customWidth="1"/>
@@ -9205,6 +9611,75 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="20">
+        <v>666677773</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="20">
+        <v>666677773</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="20">
+        <v>666677774</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
delete multiple leases from a property;set Log message from sheet;verify panel content false
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6981D0B2-5091-47F4-A926-262D9967D0B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9394F283-1FEF-4A3D-B753-3235AF556833}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="91">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -127,9 +127,6 @@
     <t>USD</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Monthly</t>
   </si>
   <si>
@@ -224,12 +221,6 @@
   </si>
   <si>
     <t>Simon</t>
-  </si>
-  <si>
-    <t>Test_Property_Auto_Final-04</t>
-  </si>
-  <si>
-    <t>Test_Property_Auto-04</t>
   </si>
   <si>
     <t>Test_Property_Auto_Final_10_Lease_Space_31</t>
@@ -777,7 +768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF54C438-284B-408F-94AA-81616ADED1B1}">
   <dimension ref="A1:AA997"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2:N6"/>
     </sheetView>
   </sheetViews>
@@ -800,7 +791,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -812,31 +803,31 @@
         <v>26</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>47</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>14</v>
@@ -857,185 +848,185 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5"/>
       <c r="D2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>56</v>
-      </c>
       <c r="F2" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" t="s">
         <v>37</v>
-      </c>
-      <c r="J2" t="s">
-        <v>38</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>25</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="5"/>
       <c r="D3" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" t="s">
         <v>37</v>
-      </c>
-      <c r="J3" t="s">
-        <v>38</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>25</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="5"/>
       <c r="D4" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" t="s">
         <v>37</v>
-      </c>
-      <c r="J4" t="s">
-        <v>38</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5"/>
       <c r="D5" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" t="s">
         <v>37</v>
-      </c>
-      <c r="J5" t="s">
-        <v>38</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>25</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="5"/>
       <c r="D6" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" t="s">
         <v>37</v>
-      </c>
-      <c r="J6" t="s">
-        <v>38</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>25</v>
@@ -1044,10 +1035,10 @@
         <v>25</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2070,7 +2061,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2112,13 +2103,13 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="Q1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>13</v>
@@ -2136,13 +2127,13 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>53</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>54</v>
       </c>
       <c r="F2" t="s">
         <v>29</v>
@@ -2160,7 +2151,7 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
@@ -2175,30 +2166,30 @@
         <v>1000</v>
       </c>
       <c r="P2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -2213,7 +2204,7 @@
         <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L3" t="s">
         <v>22</v>
@@ -2228,16 +2219,16 @@
         <v>1000</v>
       </c>
       <c r="P3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R3" t="b">
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -5239,10 +5230,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P997"/>
+  <dimension ref="A1:P996"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N6"/>
+      <selection activeCell="N2" sqref="N2:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5267,7 +5258,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -5303,7 +5294,7 @@
         <v>21</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>14</v>
@@ -5312,21 +5303,21 @@
         <v>9</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="20">
         <v>666677773</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>68</v>
@@ -5344,36 +5335,36 @@
         <v>25</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N2" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="20">
         <v>666677773</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>22</v>
@@ -5388,36 +5379,36 @@
         <v>25</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="20">
         <v>666677773</v>
       </c>
       <c r="F4" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>22</v>
@@ -5432,36 +5423,36 @@
         <v>25</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="20">
         <v>666677773</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>22</v>
@@ -5476,64 +5467,29 @@
         <v>25</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N5" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="20">
-        <v>666677774</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="A6" s="12"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
@@ -5546,12 +5502,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
@@ -5585,7 +5536,7 @@
       <c r="A16" s="12"/>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="G17" s="12"/>
     </row>
@@ -9504,10 +9455,6 @@
     <row r="996" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A996" s="12"/>
       <c r="G996" s="12"/>
-    </row>
-    <row r="997" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A997" s="12"/>
-      <c r="G997" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -9520,7 +9467,7 @@
   <dimension ref="A1:AB999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9538,7 +9485,7 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -9586,118 +9533,118 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5"/>
       <c r="D2" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="20">
         <v>666677773</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="20">
         <v>666677773</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="20">
         <v>666677773</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="20">
         <v>666677774</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="20">
         <v>666677774</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H6">
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update: 1. LeaseCreateAndSearch.java 2.PropertyCreateAndSearch.java 3.RecurringPaymentCreateandSearch.java 4.SpaceCreateAndSearch.java 5. Update compareGreaterThanValue method in UIBase.java 6.Update StoreColumnValue method in UITable ADD: 1. Add waitForRevision method in UIBase 2. Add switchLastTab and isItDigit method in UtilKeywordScript.java 3. Add chartType column in DataCreate.xlsx 4. Add steps for revision post in FASB.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478A757D-9663-4D02-8C78-D0C63C0C677C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FC94A2-1C84-4680-B865-F8DF82AB2CA7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="107">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -247,9 +247,6 @@
     <t>666677780</t>
   </si>
   <si>
-    <t>Test_Property_Auto-01</t>
-  </si>
-  <si>
     <t>Test_Property_Auto_Final-02</t>
   </si>
   <si>
@@ -286,19 +283,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>Test_Property_Auto_Final_10_Lease_Space_34</t>
-  </si>
-  <si>
     <t>1254</t>
   </si>
   <si>
-    <t>666677774</t>
-  </si>
-  <si>
     <t>Add2</t>
-  </si>
-  <si>
-    <t>Test_Property_Auto</t>
   </si>
   <si>
     <t>666677781</t>
@@ -310,14 +298,59 @@
     <t>Test_Property_Auto_Final-07</t>
   </si>
   <si>
-    <t>Test_Property_Auto_Final_10_Lease_Space_37</t>
+    <t>Test_Property_Auto_666677778</t>
+  </si>
+  <si>
+    <t>Test_Lease_666677778</t>
+  </si>
+  <si>
+    <t>Test_Lease_666677778_Space_01</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>Building List</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Owned</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>chartType</t>
+  </si>
+  <si>
+    <t>QA Testing</t>
+  </si>
+  <si>
+    <t>FASB w/o JE - FASB w/o JE Mapping</t>
+  </si>
+  <si>
+    <t>Test_667788_Propertry</t>
+  </si>
+  <si>
+    <t>667788</t>
+  </si>
+  <si>
+    <t>Test_667788_Lease</t>
+  </si>
+  <si>
+    <t>Test_667788_Lease_space</t>
+  </si>
+  <si>
+    <t>Lease_667788</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -350,6 +383,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -413,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -467,6 +518,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,7 +841,7 @@
   <dimension ref="A1:AA997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -792,7 +849,7 @@
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
     <col min="5" max="5" width="44.42578125" customWidth="1"/>
     <col min="6" max="6" width="40.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
@@ -897,7 +954,7 @@
         <v>39</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -912,7 +969,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
         <v>35</v>
@@ -933,10 +990,10 @@
         <v>48</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -951,7 +1008,7 @@
         <v>70</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
@@ -972,10 +1029,10 @@
         <v>48</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -987,10 +1044,10 @@
         <v>55</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G5" t="s">
         <v>35</v>
@@ -1011,25 +1068,25 @@
         <v>48</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>71</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="D6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>85</v>
+      <c r="D6" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
       </c>
       <c r="G6" t="s">
         <v>35</v>
@@ -1047,10 +1104,10 @@
         <v>25</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N6" s="11" t="s">
         <v>34</v>
@@ -2044,10 +2101,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2064,17 +2121,17 @@
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.140625" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" customWidth="1"/>
-    <col min="16" max="16" width="30.42578125" customWidth="1"/>
-    <col min="17" max="17" width="28.85546875" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" customWidth="1"/>
-    <col min="20" max="26" width="8.7109375" customWidth="1"/>
+    <col min="13" max="14" width="17.28515625" customWidth="1"/>
+    <col min="15" max="15" width="25.140625" customWidth="1"/>
+    <col min="16" max="16" width="32.7109375" customWidth="1"/>
+    <col min="17" max="17" width="30.42578125" customWidth="1"/>
+    <col min="18" max="18" width="28.85546875" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" customWidth="1"/>
+    <col min="20" max="20" width="17.85546875" customWidth="1"/>
+    <col min="21" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -2114,33 +2171,36 @@
       <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" s="2"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>51</v>
       </c>
@@ -2174,37 +2234,37 @@
       <c r="M2" t="s">
         <v>33</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>100000000</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>1000</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>62</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>58</v>
       </c>
-      <c r="R2" t="b">
+      <c r="S2" t="b">
         <v>1</v>
       </c>
-      <c r="S2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="T2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>89</v>
+      <c r="D3" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
         <v>30</v>
@@ -2219,7 +2279,7 @@
         <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="L3" t="s">
         <v>22</v>
@@ -2227,62 +2287,65 @@
       <c r="M3" t="s">
         <v>33</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3">
         <v>100000000</v>
       </c>
-      <c r="O3">
-        <v>1000</v>
-      </c>
       <c r="P3" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="Q3" t="s">
-        <v>58</v>
-      </c>
-      <c r="R3" t="b">
+        <v>96</v>
+      </c>
+      <c r="R3" t="s">
+        <v>97</v>
+      </c>
+      <c r="S3" t="b">
         <v>1</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -5239,7 +5302,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5247,8 +5310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P997"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5322,7 +5385,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>51</v>
       </c>
       <c r="D2" s="11" t="s">
@@ -5356,7 +5419,7 @@
         <v>66</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O2" s="14" t="s">
         <v>58</v>
@@ -5366,20 +5429,20 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="20">
-        <v>666677773</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>55</v>
+      <c r="D3" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="23">
+        <v>667788</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>104</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>22</v>
@@ -5394,16 +5457,16 @@
         <v>25</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>58</v>
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>94</v>
       </c>
       <c r="P3" s="14" t="s">
         <v>64</v>
@@ -5420,10 +5483,10 @@
         <v>666677773</v>
       </c>
       <c r="F4" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>22</v>
@@ -5444,7 +5507,7 @@
         <v>66</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O4" s="14" t="s">
         <v>58</v>
@@ -5464,10 +5527,10 @@
         <v>666677773</v>
       </c>
       <c r="F5" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>22</v>
@@ -5488,7 +5551,7 @@
         <v>66</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O5" s="14" t="s">
         <v>58</v>
@@ -5499,7 +5562,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>53</v>
@@ -5508,10 +5571,10 @@
         <v>666677774</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>22</v>
@@ -5532,7 +5595,7 @@
         <v>66</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="O6" s="14" t="s">
         <v>58</v>
@@ -9526,7 +9589,7 @@
   <dimension ref="A1:AB999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9590,28 +9653,27 @@
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="5"/>
       <c r="D2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="20">
-        <v>666677773</v>
+        <v>91</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>71</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9634,7 +9696,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9657,27 +9719,27 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="20">
-        <v>666677774</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>95</v>
+      <c r="D5" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>105</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I5" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
check UITable using contains;change OR file name
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAA7093-4B27-4CBD-AFB6-226C35555FFC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710ED78F-46A1-4CFE-9C44-EF426564BAA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="100">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -271,12 +271,6 @@
     <t>DEFAULT</t>
   </si>
   <si>
-    <t>Building List</t>
-  </si>
-  <si>
-    <t>Central</t>
-  </si>
-  <si>
     <t>Owned</t>
   </si>
   <si>
@@ -317,6 +311,18 @@
   </si>
   <si>
     <t>FASB - Charge</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>CHC</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>FASB Charge - Offshore QA FASB Charge</t>
   </si>
 </sst>
 </file>
@@ -813,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF54C438-284B-408F-94AA-81616ADED1B1}">
   <dimension ref="A1:AA997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -897,13 +903,13 @@
       </c>
       <c r="B2" s="5"/>
       <c r="D2" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>91</v>
-      </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
         <v>33</v>
@@ -1053,13 +1059,13 @@
       </c>
       <c r="B6" s="5"/>
       <c r="D6" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" t="s">
-        <v>97</v>
+        <v>93</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
@@ -1083,7 +1089,7 @@
         <v>72</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2076,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2178,10 +2184,10 @@
         <v>48</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
         <v>73</v>
@@ -2199,7 +2205,7 @@
         <v>31</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
@@ -2213,14 +2219,14 @@
       <c r="O2">
         <v>100000000</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2">
+        <v>1500</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="R2" t="s">
         <v>82</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>83</v>
-      </c>
-      <c r="R2" t="s">
-        <v>84</v>
       </c>
       <c r="S2" t="b">
         <v>1</v>
@@ -2234,10 +2240,10 @@
         <v>77</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
         <v>73</v>
@@ -2255,7 +2261,7 @@
         <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
         <v>22</v>
@@ -2269,20 +2275,20 @@
       <c r="O3">
         <v>100000000</v>
       </c>
-      <c r="P3" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>83</v>
-      </c>
-      <c r="R3" t="s">
-        <v>84</v>
+      <c r="P3">
+        <v>1500</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="S3" t="b">
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -5278,7 +5284,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5286,8 +5292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P996"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5365,16 +5371,16 @@
         <v>48</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E2" s="23">
         <v>60677888</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>22</v>
@@ -5392,7 +5398,7 @@
         <v>45</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N2" t="s">
         <v>78</v>
@@ -5409,16 +5415,16 @@
         <v>77</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="23">
         <v>60067788</v>
       </c>
       <c r="F3" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>96</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>22</v>
@@ -5435,14 +5441,14 @@
       <c r="L3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="14" t="s">
-        <v>86</v>
+      <c r="M3" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
-      </c>
-      <c r="O3" t="s">
-        <v>81</v>
+        <v>83</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="P3" s="14" t="s">
         <v>58</v>
@@ -9521,7 +9527,7 @@
   <dimension ref="A1:AB999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9590,16 +9596,16 @@
         <v>48</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>89</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>91</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -9659,22 +9665,22 @@
         <v>77</v>
       </c>
       <c r="D5" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="G5" s="24" t="s">
         <v>93</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>95</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
test data module intregation to current framework
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\AMT-TestFrameWork\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5BCB60-2443-45A2-B7C9-8D64D98F2C18}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA408F55-9647-4DD7-9EDF-8B622B2A1223}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
@@ -797,7 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF54C438-284B-408F-94AA-81616ADED1B1}">
   <dimension ref="A1:AA993"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2050,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y997"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9598,9 +9598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Insert test data from XL to database
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\AMT-TestFrameWork\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA408F55-9647-4DD7-9EDF-8B622B2A1223}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DC30BD-86DA-4246-A34C-258E565822F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
@@ -175,18 +175,6 @@
     <t>Default</t>
   </si>
   <si>
-    <t>leaseGroup1-contractTerm</t>
-  </si>
-  <si>
-    <t>propertyGroup1-buildingList</t>
-  </si>
-  <si>
-    <t>propertyGroup2-region</t>
-  </si>
-  <si>
-    <t>propertyGroup3-assetType</t>
-  </si>
-  <si>
     <t>Real Estate Contract</t>
   </si>
   <si>
@@ -293,6 +281,18 @@
   </si>
   <si>
     <t>Test_60067788_Lease_space_income_1</t>
+  </si>
+  <si>
+    <t>leaseGroup1</t>
+  </si>
+  <si>
+    <t>propertyGroup1</t>
+  </si>
+  <si>
+    <t>propertyGroup2</t>
+  </si>
+  <si>
+    <t>propertyGroup3</t>
   </si>
 </sst>
 </file>
@@ -839,7 +839,7 @@
         <v>37</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>38</v>
@@ -866,7 +866,7 @@
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -882,20 +882,20 @@
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B2" s="5"/>
       <c r="D2" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>66</v>
-      </c>
       <c r="G2" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -916,31 +916,31 @@
         <v>45</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="O2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="P2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="5"/>
       <c r="D3" s="23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -961,31 +961,31 @@
         <v>45</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="O3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="P3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B4" s="5"/>
       <c r="D4" s="23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>84</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -1006,31 +1006,31 @@
         <v>45</v>
       </c>
       <c r="N4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="O4" s="11" t="s">
-        <v>59</v>
-      </c>
       <c r="P4" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B5" s="5"/>
       <c r="D5" s="23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F5" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>84</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -1051,13 +1051,13 @@
         <v>45</v>
       </c>
       <c r="N5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="O5" s="11" t="s">
-        <v>59</v>
-      </c>
       <c r="P5" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2050,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2120,19 +2120,19 @@
         <v>11</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>13</v>
@@ -2141,7 +2141,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
@@ -2150,16 +2150,16 @@
     </row>
     <row r="2" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -2183,7 +2183,7 @@
         <v>32</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="O2">
         <v>100000000</v>
@@ -2192,33 +2192,33 @@
         <v>1500</v>
       </c>
       <c r="Q2" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="S2" t="b">
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="U2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
         <v>29</v>
@@ -2242,7 +2242,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="O3">
         <v>100000000</v>
@@ -2251,33 +2251,33 @@
         <v>1500</v>
       </c>
       <c r="Q3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="S3" t="b">
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="U3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -2292,7 +2292,7 @@
         <v>31</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L4" t="s">
         <v>22</v>
@@ -2301,42 +2301,42 @@
         <v>32</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="O4">
         <v>100000000</v>
       </c>
       <c r="P4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="Q4" s="20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="S4" t="b">
         <v>1</v>
       </c>
       <c r="T4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="U4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
         <v>29</v>
@@ -2351,7 +2351,7 @@
         <v>31</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L5" t="s">
         <v>22</v>
@@ -2360,28 +2360,28 @@
         <v>32</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="O5">
         <v>100000000</v>
       </c>
       <c r="P5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="S5" t="b">
         <v>1</v>
       </c>
       <c r="T5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="U5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -5370,8 +5370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q993"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5433,7 +5433,7 @@
         <v>21</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>14</v>
@@ -5445,24 +5445,24 @@
         <v>48</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E2" s="22">
         <v>60067788</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>22</v>
@@ -5480,36 +5480,36 @@
         <v>45</v>
       </c>
       <c r="M2" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="N2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="O2" s="14" t="s">
         <v>49</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E3" s="22">
         <v>60067788</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>22</v>
@@ -5518,7 +5518,7 @@
         <v>23</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>25</v>
@@ -5527,36 +5527,36 @@
         <v>45</v>
       </c>
       <c r="M3" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="O3" s="14" t="s">
         <v>49</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E4" s="22">
         <v>60067788</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>22</v>
@@ -5574,36 +5574,36 @@
         <v>45</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="N4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E5" s="22">
         <v>60067788</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>22</v>
@@ -5612,7 +5612,7 @@
         <v>23</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>25</v>
@@ -5621,19 +5621,19 @@
         <v>45</v>
       </c>
       <c r="M5" s="25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="N5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -9598,7 +9598,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9644,13 +9646,13 @@
         <v>28</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>43</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -9672,22 +9674,22 @@
     </row>
     <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -9699,27 +9701,27 @@
         <v>45</v>
       </c>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>71</v>
-      </c>
       <c r="G3" s="23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -9731,27 +9733,27 @@
         <v>45</v>
       </c>
       <c r="L3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -9763,27 +9765,27 @@
         <v>45</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>71</v>
-      </c>
       <c r="G5" s="23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -9795,27 +9797,27 @@
         <v>45</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>71</v>
-      </c>
       <c r="G6" s="23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -9827,7 +9829,7 @@
         <v>45</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add: Rentable lease column in db. Reslove: login issue and log message
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSI\AMTAutomationRipo\AMT-TestFrameWork\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5CA150-AF2F-4B4E-B377-1E7AD5541DA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-3780" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
@@ -18,12 +17,12 @@
     <sheet name="Lease" sheetId="3" r:id="rId3"/>
     <sheet name="Space" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="154">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -393,16 +392,116 @@
   <si>
     <t>SmokeAuto13thIn1Sp</t>
   </si>
+  <si>
+    <t>rentableLease</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -533,9 +632,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,51 +642,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -603,9 +702,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -615,64 +714,67 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{7284BA5D-4EF6-45DC-B928-7C88784A1BBA}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -983,7 +1085,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF54C438-284B-408F-94AA-81616ADED1B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3484,7 +3586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y986"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8340,10 +8442,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R981"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -13751,11 +13853,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AC983"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD983"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -13769,13 +13871,13 @@
     <col min="7" max="7" width="43.42578125" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="11" width="17.85546875" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="11"/>
-    <col min="14" max="29" width="8.7109375" customWidth="1"/>
+    <col min="10" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="11"/>
+    <col min="15" max="30" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:30">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
@@ -13809,13 +13911,15 @@
       <c r="K1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -13831,8 +13935,9 @@
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
-    </row>
-    <row r="2" spans="1:29" s="26" customFormat="1" ht="15" customHeight="1">
+      <c r="AD1" s="2"/>
+    </row>
+    <row r="2" spans="1:30" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>58</v>
       </c>
@@ -13862,14 +13967,17 @@
       <c r="K2" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="M2" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="27">
+      <c r="N2" s="27">
         <v>201480</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="26" customFormat="1" ht="15" customHeight="1">
+    <row r="3" spans="1:30" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="30" t="s">
         <v>55</v>
       </c>
@@ -13899,14 +14007,17 @@
       <c r="K3" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="M3" s="27">
+      <c r="N3" s="27">
         <v>201480</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="26" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:30" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="30" t="s">
         <v>69</v>
       </c>
@@ -13936,14 +14047,17 @@
       <c r="K4" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="M4" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="M4" s="27">
+      <c r="N4" s="27">
         <v>201480</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="26" customFormat="1" ht="15.75" customHeight="1">
+    <row r="5" spans="1:30" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="31" t="s">
         <v>70</v>
       </c>
@@ -13973,14 +14087,17 @@
       <c r="K5" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="M5" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="M5" s="27">
+      <c r="N5" s="27">
         <v>201480</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="26" customFormat="1" ht="15.75" customHeight="1">
+    <row r="6" spans="1:30" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="32">
         <v>6530957</v>
       </c>
@@ -14010,14 +14127,17 @@
       <c r="K6" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="M6" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="27">
+      <c r="N6" s="27">
         <v>201480</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="26" customFormat="1" ht="15.75" customHeight="1">
+    <row r="7" spans="1:30" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="32">
         <v>6530958</v>
       </c>
@@ -14047,14 +14167,17 @@
       <c r="K7" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="M7" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="M7" s="27">
+      <c r="N7" s="27">
         <v>201480</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="26" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:30" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="31" t="s">
         <v>73</v>
       </c>
@@ -14084,14 +14207,17 @@
       <c r="K8" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="M8" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="M8" s="27">
+      <c r="N8" s="27">
         <v>201480</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="26" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:30" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="33" t="s">
         <v>74</v>
       </c>
@@ -14121,14 +14247,17 @@
       <c r="K9" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="M9" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="M9" s="27">
+      <c r="N9" s="27">
         <v>201480</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="26" customFormat="1" ht="15.75" customHeight="1">
+    <row r="10" spans="1:30" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="32">
         <v>6551796</v>
       </c>
@@ -14158,14 +14287,17 @@
       <c r="K10" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="27" t="s">
+      <c r="L10" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="M10" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="27">
+      <c r="N10" s="27">
         <v>201480</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="26" customFormat="1" ht="15.75" customHeight="1">
+    <row r="11" spans="1:30" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="34">
         <v>6551803</v>
       </c>
@@ -14195,14 +14327,17 @@
       <c r="K11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="L11" s="27" t="s">
+      <c r="L11" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="M11" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="M11" s="27">
+      <c r="N11" s="27">
         <v>201480</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15" customHeight="1">
+    <row r="12" spans="1:30" ht="15" customHeight="1">
       <c r="A12" s="22">
         <v>6555589</v>
       </c>
@@ -14232,14 +14367,17 @@
       <c r="K12" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="M12" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>201534</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="15" customHeight="1">
+    <row r="13" spans="1:30" ht="15" customHeight="1">
       <c r="A13" s="22">
         <v>6555590</v>
       </c>
@@ -14269,14 +14407,17 @@
       <c r="K13" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L13" s="11" t="s">
+      <c r="L13" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="M13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>201534</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="15" customHeight="1">
+    <row r="14" spans="1:30" ht="15" customHeight="1">
       <c r="A14" s="22">
         <v>6530927</v>
       </c>
@@ -14306,14 +14447,17 @@
       <c r="K14" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="M14" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>201534</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1">
+    <row r="15" spans="1:30" ht="15.75" customHeight="1">
       <c r="A15" s="2">
         <v>6530966</v>
       </c>
@@ -14343,14 +14487,17 @@
       <c r="K15" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L15" s="11" t="s">
+      <c r="L15" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="M15" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>201534</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1">
+    <row r="16" spans="1:30" ht="15.75" customHeight="1">
       <c r="A16" s="2">
         <v>6530960</v>
       </c>
@@ -14380,14 +14527,17 @@
       <c r="K16" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="L16" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="M16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>201534</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1">
       <c r="A17" s="2">
         <v>6530959</v>
       </c>
@@ -14417,14 +14567,17 @@
       <c r="K17" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="L17" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="M17" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>201534</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>101</v>
       </c>
@@ -14454,14 +14607,17 @@
       <c r="K18" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L18" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="M18" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>201534</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1">
       <c r="A19" s="21">
         <v>6558241</v>
       </c>
@@ -14491,14 +14647,17 @@
       <c r="K19" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="L19" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="M19" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>201534</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1">
       <c r="A20" s="21">
         <v>6558243</v>
       </c>
@@ -14528,14 +14687,17 @@
       <c r="K20" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="M20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>201534</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1">
       <c r="A21" s="21">
         <v>6558245</v>
       </c>
@@ -14565,14 +14727,17 @@
       <c r="K21" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="L21" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="M21" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>201534</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1">
       <c r="A22" s="22">
         <v>6555587</v>
       </c>
@@ -14602,14 +14767,17 @@
       <c r="K22" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="L22" s="39" t="s">
+      <c r="L22" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="M22" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="M22" s="42">
+      <c r="N22" s="42">
         <v>201536</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1">
       <c r="A23" s="22">
         <v>6555588</v>
       </c>
@@ -14639,14 +14807,17 @@
       <c r="K23" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="L23" s="39" t="s">
+      <c r="L23" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="M23" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="M23" s="42">
+      <c r="N23" s="42">
         <v>201536</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1">
       <c r="A24" s="43" t="s">
         <v>113</v>
       </c>
@@ -14676,14 +14847,17 @@
       <c r="K24" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="L24" s="39" t="s">
+      <c r="L24" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="M24" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="M24" s="42">
+      <c r="N24" s="42">
         <v>201536</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1">
       <c r="A25" s="44" t="s">
         <v>114</v>
       </c>
@@ -14713,14 +14887,17 @@
       <c r="K25" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="L25" s="39" t="s">
+      <c r="L25" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="M25" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="M25" s="42">
+      <c r="N25" s="42">
         <v>201536</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1">
+    <row r="26" spans="1:14" ht="15.75" customHeight="1">
       <c r="A26" s="45" t="s">
         <v>115</v>
       </c>
@@ -14750,14 +14927,17 @@
       <c r="K26" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="L26" s="39" t="s">
+      <c r="L26" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="M26" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="M26" s="42">
+      <c r="N26" s="42">
         <v>201536</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" s="45" t="s">
         <v>118</v>
       </c>
@@ -14787,14 +14967,17 @@
       <c r="K27" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="L27" s="39" t="s">
+      <c r="L27" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="M27" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="M27" s="42">
+      <c r="N27" s="42">
         <v>201536</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="21">
         <v>6541329</v>
       </c>
@@ -14824,14 +15007,17 @@
       <c r="K28" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="L28" s="39" t="s">
+      <c r="L28" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="M28" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="M28" s="42">
+      <c r="N28" s="42">
         <v>201536</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" s="21">
         <v>6558247</v>
       </c>
@@ -14861,14 +15047,17 @@
       <c r="K29" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="L29" s="39" t="s">
+      <c r="L29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="M29" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="M29" s="42">
+      <c r="N29" s="42">
         <v>201536</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1">
       <c r="A30" s="21">
         <v>6558248</v>
       </c>
@@ -14898,14 +15087,17 @@
       <c r="K30" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="L30" s="39" t="s">
+      <c r="L30" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="M30" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="M30" s="42">
+      <c r="N30" s="42">
         <v>201536</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.75" customHeight="1">
+    <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="2">
         <v>6558250</v>
       </c>
@@ -14935,14 +15127,17 @@
       <c r="K31" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="L31" s="39" t="s">
+      <c r="L31" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="M31" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="M31" s="42">
+      <c r="N31" s="42">
         <v>201536</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Resolve post issue for App env
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="183">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -552,7 +552,25 @@
     <t>FASB1</t>
   </si>
   <si>
-    <t>SmokePostEInSp601</t>
+    <t>Post Revision</t>
+  </si>
+  <si>
+    <t>Add Revision</t>
+  </si>
+  <si>
+    <t>SmokeAddCal</t>
+  </si>
+  <si>
+    <t>Post revision</t>
+  </si>
+  <si>
+    <t>Add revision</t>
+  </si>
+  <si>
+    <t>SmokeAddEx489</t>
+  </si>
+  <si>
+    <t>SmokeAddExSp489</t>
   </si>
 </sst>
 </file>
@@ -621,11 +639,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -639,7 +659,7 @@
       <name val="Docs-Lato"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -724,8 +744,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -819,12 +851,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -981,7 +1055,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1002,7 +1075,6 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1082,6 +1154,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1399,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA989"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F25" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1524,8 +1628,8 @@
       <c r="N2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="33" t="s">
-        <v>54</v>
+      <c r="O2" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>140</v>
@@ -1574,8 +1678,8 @@
       <c r="N3" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="33" t="s">
-        <v>54</v>
+      <c r="O3" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P3" s="19" t="s">
         <v>140</v>
@@ -1624,8 +1728,8 @@
       <c r="N4" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="33" t="s">
-        <v>54</v>
+      <c r="O4" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P4" s="19" t="s">
         <v>140</v>
@@ -1674,8 +1778,8 @@
       <c r="N5" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="33" t="s">
-        <v>54</v>
+      <c r="O5" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P5" s="19" t="s">
         <v>140</v>
@@ -1724,8 +1828,8 @@
       <c r="N6" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="33" t="s">
-        <v>54</v>
+      <c r="O6" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P6" s="19" t="s">
         <v>140</v>
@@ -1774,8 +1878,8 @@
       <c r="N7" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O7" s="33" t="s">
-        <v>54</v>
+      <c r="O7" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P7" s="19" t="s">
         <v>140</v>
@@ -1824,8 +1928,8 @@
       <c r="N8" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="33" t="s">
-        <v>54</v>
+      <c r="O8" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P8" s="19" t="s">
         <v>140</v>
@@ -1874,8 +1978,8 @@
       <c r="N9" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O9" s="33" t="s">
-        <v>54</v>
+      <c r="O9" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P9" s="19" t="s">
         <v>140</v>
@@ -1924,8 +2028,8 @@
       <c r="N10" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="33" t="s">
-        <v>54</v>
+      <c r="O10" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P10" s="19" t="s">
         <v>140</v>
@@ -1974,8 +2078,8 @@
       <c r="N11" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="O11" s="33" t="s">
-        <v>54</v>
+      <c r="O11" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P11" s="19" t="s">
         <v>140</v>
@@ -2023,8 +2127,8 @@
       <c r="N12" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O12" s="10" t="s">
-        <v>54</v>
+      <c r="O12" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P12" s="19" t="s">
         <v>140</v>
@@ -2071,8 +2175,8 @@
       <c r="N13" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O13" s="10" t="s">
-        <v>54</v>
+      <c r="O13" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P13" s="19" t="s">
         <v>140</v>
@@ -2119,8 +2223,8 @@
       <c r="N14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O14" s="10" t="s">
-        <v>54</v>
+      <c r="O14" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P14" s="19" t="s">
         <v>140</v>
@@ -2167,8 +2271,8 @@
       <c r="N15" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O15" s="10" t="s">
-        <v>54</v>
+      <c r="O15" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P15" s="19" t="s">
         <v>140</v>
@@ -2215,8 +2319,8 @@
       <c r="N16" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O16" s="10" t="s">
-        <v>54</v>
+      <c r="O16" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P16" s="19" t="s">
         <v>140</v>
@@ -2263,8 +2367,8 @@
       <c r="N17" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O17" s="10" t="s">
-        <v>54</v>
+      <c r="O17" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P17" s="19" t="s">
         <v>140</v>
@@ -2311,8 +2415,8 @@
       <c r="N18" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O18" s="10" t="s">
-        <v>54</v>
+      <c r="O18" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P18" s="19" t="s">
         <v>140</v>
@@ -2359,8 +2463,8 @@
       <c r="N19" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O19" s="10" t="s">
-        <v>54</v>
+      <c r="O19" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P19" s="19" t="s">
         <v>140</v>
@@ -2407,8 +2511,8 @@
       <c r="N20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O20" s="10" t="s">
-        <v>54</v>
+      <c r="O20" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P20" s="19" t="s">
         <v>140</v>
@@ -2454,8 +2558,8 @@
       <c r="N21" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O21" s="10" t="s">
-        <v>54</v>
+      <c r="O21" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="P21" s="19" t="s">
         <v>140</v>
@@ -2504,7 +2608,7 @@
         <v>50</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P22" s="19" t="s">
         <v>140</v>
@@ -2553,7 +2657,7 @@
         <v>50</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P23" s="19" t="s">
         <v>140</v>
@@ -2602,7 +2706,7 @@
         <v>50</v>
       </c>
       <c r="O24" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P24" s="19" t="s">
         <v>140</v>
@@ -2651,7 +2755,7 @@
         <v>50</v>
       </c>
       <c r="O25" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P25" s="19" t="s">
         <v>140</v>
@@ -2700,7 +2804,7 @@
         <v>50</v>
       </c>
       <c r="O26" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P26" s="19" t="s">
         <v>140</v>
@@ -2749,7 +2853,7 @@
         <v>50</v>
       </c>
       <c r="O27" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P27" s="19" t="s">
         <v>140</v>
@@ -2798,7 +2902,7 @@
         <v>50</v>
       </c>
       <c r="O28" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P28" s="19" t="s">
         <v>140</v>
@@ -2847,7 +2951,7 @@
         <v>50</v>
       </c>
       <c r="O29" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P29" s="19" t="s">
         <v>140</v>
@@ -2896,7 +3000,7 @@
         <v>50</v>
       </c>
       <c r="O30" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P30" s="19" t="s">
         <v>140</v>
@@ -2945,7 +3049,7 @@
         <v>50</v>
       </c>
       <c r="O31" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P31" s="19" t="s">
         <v>140</v>
@@ -2954,8 +3058,24 @@
         <v>201482</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="33" spans="1:17" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="32" spans="1:17" ht="15.75" customHeight="1">
+      <c r="O32" s="139" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" s="128" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B33" s="137" t="s">
+        <v>176</v>
+      </c>
+      <c r="C33" s="129"/>
+      <c r="D33" s="129"/>
+      <c r="E33" s="129"/>
+      <c r="F33" s="129"/>
+      <c r="G33" s="129"/>
+      <c r="O33" s="136" t="s">
+        <v>173</v>
+      </c>
+    </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
       <c r="A34" s="83">
         <v>6519011</v>
@@ -2995,8 +3115,8 @@
       <c r="N34" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="O34" s="30" t="s">
-        <v>54</v>
+      <c r="O34" s="136" t="s">
+        <v>173</v>
       </c>
       <c r="P34" s="29" t="s">
         <v>145</v>
@@ -3006,7 +3126,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A35" s="89">
+      <c r="A35" s="88">
         <v>6519013</v>
       </c>
       <c r="B35" s="28"/>
@@ -3044,8 +3164,8 @@
       <c r="N35" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="O35" s="30" t="s">
-        <v>54</v>
+      <c r="O35" s="136" t="s">
+        <v>173</v>
       </c>
       <c r="P35" s="29" t="s">
         <v>145</v>
@@ -3055,12 +3175,12 @@
       </c>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A36" s="90">
+      <c r="A36" s="89">
         <v>6596696</v>
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="28"/>
-      <c r="D36" s="91" t="s">
+      <c r="D36" s="90" t="s">
         <v>148</v>
       </c>
       <c r="E36" s="84" t="s">
@@ -3093,8 +3213,8 @@
       <c r="N36" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="O36" s="30" t="s">
-        <v>54</v>
+      <c r="O36" s="136" t="s">
+        <v>173</v>
       </c>
       <c r="P36" s="29" t="s">
         <v>145</v>
@@ -3104,12 +3224,12 @@
       </c>
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A37" s="90">
+      <c r="A37" s="89">
         <v>6596733</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
-      <c r="D37" s="91" t="s">
+      <c r="D37" s="90" t="s">
         <v>150</v>
       </c>
       <c r="E37" s="84" t="s">
@@ -3142,8 +3262,8 @@
       <c r="N37" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="O37" s="30" t="s">
-        <v>54</v>
+      <c r="O37" s="136" t="s">
+        <v>173</v>
       </c>
       <c r="P37" s="29" t="s">
         <v>145</v>
@@ -3154,7 +3274,7 @@
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
       <c r="A38" s="17"/>
-      <c r="B38" s="128"/>
+      <c r="B38" s="126"/>
       <c r="C38" s="18"/>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
@@ -3164,15 +3284,17 @@
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
       <c r="K38" s="18"/>
-      <c r="L38" s="120"/>
-      <c r="M38" s="120"/>
-      <c r="N38" s="120"/>
-      <c r="O38" s="120"/>
+      <c r="L38" s="118"/>
+      <c r="M38" s="118"/>
+      <c r="N38" s="118"/>
+      <c r="O38" s="136" t="s">
+        <v>173</v>
+      </c>
       <c r="P38" s="19"/>
       <c r="Q38" s="18"/>
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A39" s="116">
+      <c r="A39" s="114">
         <v>6596575</v>
       </c>
       <c r="B39" s="28"/>
@@ -3210,18 +3332,18 @@
       <c r="N39" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="O39" s="30" t="s">
-        <v>54</v>
+      <c r="O39" s="136" t="s">
+        <v>173</v>
       </c>
       <c r="P39" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="Q39" s="102">
+      <c r="Q39" s="100">
         <v>201534</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A40" s="116">
+      <c r="A40" s="114">
         <v>6596601</v>
       </c>
       <c r="B40" s="28"/>
@@ -3230,7 +3352,7 @@
         <v>155</v>
       </c>
       <c r="E40" s="84" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>174</v>
@@ -3259,18 +3381,18 @@
       <c r="N40" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="O40" s="30" t="s">
+      <c r="O40" s="140" t="s">
         <v>54</v>
       </c>
       <c r="P40" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="Q40" s="102">
+      <c r="Q40" s="100">
         <v>201534</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A41" s="116">
+      <c r="A41" s="114">
         <v>6596609</v>
       </c>
       <c r="B41" s="28"/>
@@ -3309,17 +3431,17 @@
         <v>50</v>
       </c>
       <c r="O41" s="30" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P41" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="Q41" s="102">
+      <c r="Q41" s="100">
         <v>201534</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A42" s="116">
+      <c r="A42" s="114">
         <v>6596613</v>
       </c>
       <c r="B42" s="28"/>
@@ -3358,12 +3480,12 @@
         <v>50</v>
       </c>
       <c r="O42" s="30" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P42" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="Q42" s="102">
+      <c r="Q42" s="100">
         <v>201534</v>
       </c>
     </row>
@@ -3379,7 +3501,9 @@
       <c r="L43" s="11"/>
       <c r="M43" s="11"/>
       <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
+      <c r="O43" s="30" t="s">
+        <v>173</v>
+      </c>
       <c r="P43" s="10"/>
     </row>
     <row r="44" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
@@ -3412,7 +3536,7 @@
       <c r="K44" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="L44" s="101" t="s">
+      <c r="L44" s="99" t="s">
         <v>164</v>
       </c>
       <c r="M44" s="30" t="s">
@@ -3422,17 +3546,17 @@
         <v>50</v>
       </c>
       <c r="O44" s="30" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P44" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="Q44" s="102">
+      <c r="Q44" s="100">
         <v>201536</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A45" s="89">
+      <c r="A45" s="88">
         <v>6596619</v>
       </c>
       <c r="B45" s="28"/>
@@ -3461,7 +3585,7 @@
       <c r="K45" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="L45" s="101" t="s">
+      <c r="L45" s="99" t="s">
         <v>164</v>
       </c>
       <c r="M45" s="30" t="s">
@@ -3471,22 +3595,22 @@
         <v>50</v>
       </c>
       <c r="O45" s="30" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P45" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="Q45" s="102">
+      <c r="Q45" s="100">
         <v>201536</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A46" s="89">
+      <c r="A46" s="88">
         <v>6596630</v>
       </c>
       <c r="B46" s="28"/>
       <c r="C46" s="28"/>
-      <c r="D46" s="91" t="s">
+      <c r="D46" s="90" t="s">
         <v>168</v>
       </c>
       <c r="E46" s="84" t="s">
@@ -3510,7 +3634,7 @@
       <c r="K46" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="L46" s="101" t="s">
+      <c r="L46" s="99" t="s">
         <v>164</v>
       </c>
       <c r="M46" s="30" t="s">
@@ -3520,22 +3644,22 @@
         <v>50</v>
       </c>
       <c r="O46" s="30" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P46" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="Q46" s="102">
+      <c r="Q46" s="100">
         <v>201536</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A47" s="89">
+      <c r="A47" s="88">
         <v>6596686</v>
       </c>
       <c r="B47" s="28"/>
       <c r="C47" s="28"/>
-      <c r="D47" s="91" t="s">
+      <c r="D47" s="90" t="s">
         <v>170</v>
       </c>
       <c r="E47" s="84" t="s">
@@ -3559,7 +3683,7 @@
       <c r="K47" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="L47" s="101" t="s">
+      <c r="L47" s="99" t="s">
         <v>164</v>
       </c>
       <c r="M47" s="30" t="s">
@@ -3569,32 +3693,96 @@
         <v>50</v>
       </c>
       <c r="O47" s="30" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="P47" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="Q47" s="102">
+      <c r="Q47" s="100">
         <v>201536</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:17" ht="15.75" customHeight="1">
+      <c r="O48" s="30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" s="128" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B49" s="137" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="129"/>
+      <c r="D49" s="129"/>
+      <c r="E49" s="129"/>
+      <c r="F49" s="129"/>
+      <c r="G49" s="129"/>
+      <c r="O49" s="30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A50" s="134">
+        <v>6579489</v>
+      </c>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="E50" s="84" t="s">
+        <v>182</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="H50" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I50" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J50" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="K50" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="L50" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="N50" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="O50" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="P50" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q50" s="28">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="52" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="53" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="54" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="55" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="56" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="57" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="58" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="59" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="60" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="61" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="62" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="63" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="64" spans="1:17" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -4521,6 +4709,10 @@
     <row r="988" ht="15.75" customHeight="1"/>
     <row r="989" ht="15.75" customHeight="1"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B49:G49"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4530,8 +4722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y986"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4683,8 +4875,8 @@
       <c r="S2" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="T2" s="19" t="s">
-        <v>54</v>
+      <c r="T2" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U2" s="19" t="s">
         <v>140</v>
@@ -4745,8 +4937,8 @@
       <c r="S3" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="T3" s="19" t="s">
-        <v>54</v>
+      <c r="T3" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U3" s="19" t="s">
         <v>140</v>
@@ -4807,8 +4999,8 @@
       <c r="S4" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="T4" s="19" t="s">
-        <v>54</v>
+      <c r="T4" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U4" s="19" t="s">
         <v>140</v>
@@ -4869,8 +5061,8 @@
       <c r="S5" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="T5" s="19" t="s">
-        <v>54</v>
+      <c r="T5" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U5" s="19" t="s">
         <v>140</v>
@@ -4931,8 +5123,8 @@
       <c r="S6" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="T6" s="19" t="s">
-        <v>54</v>
+      <c r="T6" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U6" s="19" t="s">
         <v>140</v>
@@ -4993,8 +5185,8 @@
       <c r="S7" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="T7" s="19" t="s">
-        <v>54</v>
+      <c r="T7" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U7" s="19" t="s">
         <v>140</v>
@@ -5055,8 +5247,8 @@
       <c r="S8" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="T8" s="19" t="s">
-        <v>54</v>
+      <c r="T8" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U8" s="19" t="s">
         <v>140</v>
@@ -5117,8 +5309,8 @@
       <c r="S9" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="T9" s="19" t="s">
-        <v>54</v>
+      <c r="T9" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U9" s="19" t="s">
         <v>140</v>
@@ -5179,8 +5371,8 @@
       <c r="S10" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="T10" s="19" t="s">
-        <v>54</v>
+      <c r="T10" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U10" s="19" t="s">
         <v>140</v>
@@ -5241,8 +5433,8 @@
       <c r="S11" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="T11" s="19" t="s">
-        <v>54</v>
+      <c r="T11" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U11" s="19" t="s">
         <v>140</v>
@@ -5303,8 +5495,8 @@
       <c r="S12" t="b">
         <v>1</v>
       </c>
-      <c r="T12" s="10" t="s">
-        <v>54</v>
+      <c r="T12" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U12" s="19" t="s">
         <v>140</v>
@@ -5365,8 +5557,8 @@
       <c r="S13" t="b">
         <v>1</v>
       </c>
-      <c r="T13" s="10" t="s">
-        <v>54</v>
+      <c r="T13" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U13" s="19" t="s">
         <v>140</v>
@@ -5427,8 +5619,8 @@
       <c r="S14" t="b">
         <v>1</v>
       </c>
-      <c r="T14" s="10" t="s">
-        <v>54</v>
+      <c r="T14" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U14" s="19" t="s">
         <v>140</v>
@@ -5489,8 +5681,8 @@
       <c r="S15" t="b">
         <v>1</v>
       </c>
-      <c r="T15" s="10" t="s">
-        <v>54</v>
+      <c r="T15" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U15" s="19" t="s">
         <v>140</v>
@@ -5551,8 +5743,8 @@
       <c r="S16" t="b">
         <v>1</v>
       </c>
-      <c r="T16" s="10" t="s">
-        <v>54</v>
+      <c r="T16" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U16" s="19" t="s">
         <v>140</v>
@@ -5613,8 +5805,8 @@
       <c r="S17" t="b">
         <v>1</v>
       </c>
-      <c r="T17" s="10" t="s">
-        <v>54</v>
+      <c r="T17" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U17" s="19" t="s">
         <v>140</v>
@@ -5675,8 +5867,8 @@
       <c r="S18" t="b">
         <v>1</v>
       </c>
-      <c r="T18" s="10" t="s">
-        <v>54</v>
+      <c r="T18" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U18" s="19" t="s">
         <v>140</v>
@@ -5737,8 +5929,8 @@
       <c r="S19" t="b">
         <v>1</v>
       </c>
-      <c r="T19" s="10" t="s">
-        <v>54</v>
+      <c r="T19" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U19" s="19" t="s">
         <v>140</v>
@@ -5799,8 +5991,8 @@
       <c r="S20" t="b">
         <v>1</v>
       </c>
-      <c r="T20" s="10" t="s">
-        <v>54</v>
+      <c r="T20" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U20" s="19" t="s">
         <v>140</v>
@@ -5861,8 +6053,8 @@
       <c r="S21" t="b">
         <v>1</v>
       </c>
-      <c r="T21" s="10" t="s">
-        <v>54</v>
+      <c r="T21" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="U21" s="19" t="s">
         <v>140</v>
@@ -5926,7 +6118,7 @@
         <v>1</v>
       </c>
       <c r="T22" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U22" s="19" t="s">
         <v>140</v>
@@ -5990,7 +6182,7 @@
         <v>1</v>
       </c>
       <c r="T23" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U23" s="19" t="s">
         <v>140</v>
@@ -6054,7 +6246,7 @@
         <v>1</v>
       </c>
       <c r="T24" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U24" s="19" t="s">
         <v>140</v>
@@ -6118,7 +6310,7 @@
         <v>1</v>
       </c>
       <c r="T25" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U25" s="19" t="s">
         <v>140</v>
@@ -6182,7 +6374,7 @@
         <v>1</v>
       </c>
       <c r="T26" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U26" s="19" t="s">
         <v>140</v>
@@ -6246,7 +6438,7 @@
         <v>1</v>
       </c>
       <c r="T27" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U27" s="19" t="s">
         <v>140</v>
@@ -6310,7 +6502,7 @@
         <v>1</v>
       </c>
       <c r="T28" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U28" s="19" t="s">
         <v>140</v>
@@ -6374,7 +6566,7 @@
         <v>1</v>
       </c>
       <c r="T29" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U29" s="19" t="s">
         <v>140</v>
@@ -6438,7 +6630,7 @@
         <v>1</v>
       </c>
       <c r="T30" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U30" s="19" t="s">
         <v>140</v>
@@ -6502,7 +6694,7 @@
         <v>1</v>
       </c>
       <c r="T31" s="21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U31" s="19" t="s">
         <v>140</v>
@@ -6511,8 +6703,19 @@
         <v>201482</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A32" s="4"/>
+    <row r="32" spans="1:22" s="128" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A32" s="127"/>
+      <c r="B32" s="131" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="130"/>
+      <c r="D32" s="130"/>
+      <c r="E32" s="130"/>
+      <c r="F32" s="130"/>
+      <c r="G32" s="130"/>
+      <c r="T32" s="136" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A33" s="83">
@@ -6535,7 +6738,7 @@
       <c r="H33" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I33" s="117">
+      <c r="I33" s="115">
         <v>12230</v>
       </c>
       <c r="J33" s="85" t="s">
@@ -6550,36 +6753,36 @@
       <c r="M33" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N33" s="124" t="s">
+      <c r="N33" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O33" s="117">
+      <c r="O33" s="115">
         <v>100000000</v>
       </c>
       <c r="P33" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q33" s="124" t="s">
+      <c r="Q33" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="R33" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="S33" s="125" t="b">
+      <c r="R33" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="S33" s="123" t="b">
         <v>1</v>
       </c>
       <c r="T33" s="85" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U33" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V33" s="117">
-        <v>201534</v>
+      <c r="V33" s="115">
+        <v>201480</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A34" s="89">
+      <c r="A34" s="88">
         <v>6519013</v>
       </c>
       <c r="B34" s="85"/>
@@ -6599,7 +6802,7 @@
       <c r="H34" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I34" s="117">
+      <c r="I34" s="115">
         <v>12230</v>
       </c>
       <c r="J34" s="85" t="s">
@@ -6614,36 +6817,36 @@
       <c r="M34" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N34" s="124" t="s">
+      <c r="N34" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O34" s="117">
+      <c r="O34" s="115">
         <v>100000000</v>
       </c>
       <c r="P34" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q34" s="124" t="s">
+      <c r="Q34" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="R34" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="S34" s="125" t="b">
+      <c r="R34" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="S34" s="123" t="b">
         <v>1</v>
       </c>
       <c r="T34" s="85" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U34" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V34" s="117">
-        <v>201534</v>
+      <c r="V34" s="115">
+        <v>201480</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A35" s="90">
+      <c r="A35" s="89">
         <v>6596696</v>
       </c>
       <c r="B35" s="85"/>
@@ -6663,7 +6866,7 @@
       <c r="H35" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="117">
+      <c r="I35" s="115">
         <v>12230</v>
       </c>
       <c r="J35" s="85" t="s">
@@ -6678,36 +6881,36 @@
       <c r="M35" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N35" s="124" t="s">
+      <c r="N35" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O35" s="117">
+      <c r="O35" s="115">
         <v>100000000</v>
       </c>
       <c r="P35" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q35" s="124" t="s">
+      <c r="Q35" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="R35" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="S35" s="125" t="b">
+      <c r="R35" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="S35" s="123" t="b">
         <v>1</v>
       </c>
       <c r="T35" s="85" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U35" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V35" s="117">
-        <v>201534</v>
+      <c r="V35" s="115">
+        <v>201480</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A36" s="90">
+      <c r="A36" s="89">
         <v>6596733</v>
       </c>
       <c r="B36" s="85"/>
@@ -6727,7 +6930,7 @@
       <c r="H36" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="117">
+      <c r="I36" s="115">
         <v>12230</v>
       </c>
       <c r="J36" s="85" t="s">
@@ -6742,36 +6945,36 @@
       <c r="M36" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N36" s="124" t="s">
+      <c r="N36" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O36" s="117">
+      <c r="O36" s="115">
         <v>100000000</v>
       </c>
       <c r="P36" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q36" s="124" t="s">
+      <c r="Q36" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="R36" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="S36" s="125" t="b">
+      <c r="R36" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="S36" s="123" t="b">
         <v>1</v>
       </c>
       <c r="T36" s="85" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U36" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V36" s="117">
-        <v>201534</v>
+      <c r="V36" s="115">
+        <v>201480</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A37" s="126"/>
+      <c r="A37" s="124"/>
       <c r="B37" s="85"/>
       <c r="C37" s="85"/>
       <c r="D37" s="85"/>
@@ -6779,23 +6982,25 @@
       <c r="F37" s="85"/>
       <c r="G37" s="85"/>
       <c r="H37" s="85"/>
-      <c r="I37" s="117"/>
+      <c r="I37" s="115"/>
       <c r="J37" s="85"/>
       <c r="K37" s="85"/>
       <c r="L37" s="85"/>
       <c r="M37" s="85"/>
-      <c r="N37" s="124"/>
-      <c r="O37" s="117"/>
+      <c r="N37" s="122"/>
+      <c r="O37" s="115"/>
       <c r="P37" s="85"/>
-      <c r="Q37" s="124"/>
+      <c r="Q37" s="122"/>
       <c r="R37" s="85"/>
-      <c r="S37" s="125"/>
-      <c r="T37" s="85"/>
+      <c r="S37" s="123"/>
+      <c r="T37" s="85" t="s">
+        <v>173</v>
+      </c>
       <c r="U37" s="85"/>
-      <c r="V37" s="117"/>
+      <c r="V37" s="115"/>
     </row>
     <row r="38" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A38" s="116">
+      <c r="A38" s="114">
         <v>6596575</v>
       </c>
       <c r="B38" s="85"/>
@@ -6815,7 +7020,7 @@
       <c r="H38" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I38" s="117">
+      <c r="I38" s="115">
         <v>12230</v>
       </c>
       <c r="J38" s="85" t="s">
@@ -6830,36 +7035,36 @@
       <c r="M38" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N38" s="124" t="s">
+      <c r="N38" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O38" s="117">
+      <c r="O38" s="115">
         <v>100000000</v>
       </c>
       <c r="P38" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q38" s="124" t="s">
+      <c r="Q38" s="122" t="s">
         <v>62</v>
       </c>
       <c r="R38" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S38" s="125" t="b">
+      <c r="S38" s="123" t="b">
         <v>1</v>
       </c>
       <c r="T38" s="85" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="U38" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V38" s="117">
+      <c r="V38" s="115">
         <v>201534</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A39" s="116">
+      <c r="A39" s="114">
         <v>6596601</v>
       </c>
       <c r="B39" s="85"/>
@@ -6879,7 +7084,7 @@
       <c r="H39" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I39" s="117">
+      <c r="I39" s="115">
         <v>12230</v>
       </c>
       <c r="J39" s="85" t="s">
@@ -6894,36 +7099,36 @@
       <c r="M39" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N39" s="124" t="s">
+      <c r="N39" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O39" s="117">
+      <c r="O39" s="115">
         <v>100000000</v>
       </c>
       <c r="P39" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q39" s="124" t="s">
+      <c r="Q39" s="122" t="s">
         <v>62</v>
       </c>
       <c r="R39" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S39" s="125" t="b">
+      <c r="S39" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="T39" s="85" t="s">
+      <c r="T39" s="141" t="s">
         <v>54</v>
       </c>
       <c r="U39" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V39" s="117">
+      <c r="V39" s="115">
         <v>201534</v>
       </c>
     </row>
     <row r="40" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A40" s="116">
+      <c r="A40" s="114">
         <v>6596609</v>
       </c>
       <c r="B40" s="85"/>
@@ -6943,7 +7148,7 @@
       <c r="H40" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I40" s="117">
+      <c r="I40" s="115">
         <v>12230</v>
       </c>
       <c r="J40" s="85" t="s">
@@ -6958,36 +7163,36 @@
       <c r="M40" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N40" s="124" t="s">
+      <c r="N40" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O40" s="117">
+      <c r="O40" s="115">
         <v>100000000</v>
       </c>
       <c r="P40" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q40" s="124" t="s">
+      <c r="Q40" s="122" t="s">
         <v>62</v>
       </c>
       <c r="R40" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S40" s="125" t="b">
+      <c r="S40" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="T40" s="85" t="s">
-        <v>54</v>
+      <c r="T40" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="U40" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V40" s="117">
+      <c r="V40" s="115">
         <v>201534</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A41" s="116">
+      <c r="A41" s="114">
         <v>6596613</v>
       </c>
       <c r="B41" s="85"/>
@@ -7007,7 +7212,7 @@
       <c r="H41" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I41" s="117">
+      <c r="I41" s="115">
         <v>12230</v>
       </c>
       <c r="J41" s="85" t="s">
@@ -7022,31 +7227,31 @@
       <c r="M41" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N41" s="124" t="s">
+      <c r="N41" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O41" s="117">
+      <c r="O41" s="115">
         <v>100000000</v>
       </c>
       <c r="P41" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q41" s="124" t="s">
+      <c r="Q41" s="122" t="s">
         <v>62</v>
       </c>
       <c r="R41" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S41" s="125" t="b">
+      <c r="S41" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="T41" s="85" t="s">
-        <v>54</v>
+      <c r="T41" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="U41" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V41" s="117">
+      <c r="V41" s="115">
         <v>201534</v>
       </c>
     </row>
@@ -7070,9 +7275,11 @@
       <c r="Q42" s="20"/>
       <c r="R42" s="19"/>
       <c r="S42" s="18"/>
-      <c r="T42" s="19"/>
+      <c r="T42" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="U42" s="18"/>
-      <c r="V42" s="127"/>
+      <c r="V42" s="125"/>
     </row>
     <row r="43" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
       <c r="A43" s="83">
@@ -7095,7 +7302,7 @@
       <c r="H43" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I43" s="117">
+      <c r="I43" s="115">
         <v>12230</v>
       </c>
       <c r="J43" s="85" t="s">
@@ -7110,36 +7317,36 @@
       <c r="M43" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N43" s="124" t="s">
+      <c r="N43" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O43" s="117">
+      <c r="O43" s="115">
         <v>100000000</v>
       </c>
       <c r="P43" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q43" s="124" t="s">
+      <c r="Q43" s="122" t="s">
         <v>62</v>
       </c>
       <c r="R43" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S43" s="125" t="b">
+      <c r="S43" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="T43" s="85" t="s">
+      <c r="T43" s="19" t="s">
         <v>173</v>
       </c>
       <c r="U43" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V43" s="117">
+      <c r="V43" s="115">
         <v>201536</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A44" s="89">
+      <c r="A44" s="88">
         <v>6596619</v>
       </c>
       <c r="B44" s="85"/>
@@ -7159,7 +7366,7 @@
       <c r="H44" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I44" s="117">
+      <c r="I44" s="115">
         <v>12230</v>
       </c>
       <c r="J44" s="85" t="s">
@@ -7174,36 +7381,36 @@
       <c r="M44" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N44" s="124" t="s">
+      <c r="N44" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O44" s="117">
+      <c r="O44" s="115">
         <v>100000000</v>
       </c>
       <c r="P44" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q44" s="124" t="s">
+      <c r="Q44" s="122" t="s">
         <v>62</v>
       </c>
       <c r="R44" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S44" s="125" t="b">
+      <c r="S44" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="T44" s="85" t="s">
-        <v>54</v>
+      <c r="T44" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="U44" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V44" s="117">
+      <c r="V44" s="115">
         <v>201536</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A45" s="89">
+      <c r="A45" s="88">
         <v>6596630</v>
       </c>
       <c r="B45" s="85"/>
@@ -7223,7 +7430,7 @@
       <c r="H45" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I45" s="117">
+      <c r="I45" s="115">
         <v>12230</v>
       </c>
       <c r="J45" s="85" t="s">
@@ -7238,36 +7445,36 @@
       <c r="M45" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N45" s="124" t="s">
+      <c r="N45" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O45" s="117">
+      <c r="O45" s="115">
         <v>100000000</v>
       </c>
       <c r="P45" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q45" s="124" t="s">
+      <c r="Q45" s="122" t="s">
         <v>62</v>
       </c>
       <c r="R45" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S45" s="125" t="b">
+      <c r="S45" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="T45" s="85" t="s">
-        <v>54</v>
+      <c r="T45" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="U45" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V45" s="117">
+      <c r="V45" s="115">
         <v>201536</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A46" s="89">
+      <c r="A46" s="88">
         <v>6596686</v>
       </c>
       <c r="B46" s="85"/>
@@ -7287,7 +7494,7 @@
       <c r="H46" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I46" s="117">
+      <c r="I46" s="115">
         <v>12230</v>
       </c>
       <c r="J46" s="85" t="s">
@@ -7302,39 +7509,113 @@
       <c r="M46" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="N46" s="124" t="s">
+      <c r="N46" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="O46" s="117">
+      <c r="O46" s="115">
         <v>100000000</v>
       </c>
       <c r="P46" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="Q46" s="124" t="s">
+      <c r="Q46" s="122" t="s">
         <v>62</v>
       </c>
       <c r="R46" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S46" s="125" t="b">
+      <c r="S46" s="123" t="b">
         <v>1</v>
       </c>
-      <c r="T46" s="85" t="s">
-        <v>54</v>
+      <c r="T46" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="U46" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="V46" s="117">
+      <c r="V46" s="115">
         <v>201536</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A47" s="4"/>
-    </row>
-    <row r="48" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A48" s="4"/>
+    <row r="47" spans="1:22" s="128" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A47" s="127"/>
+      <c r="B47" s="133" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="132"/>
+      <c r="D47" s="132"/>
+      <c r="E47" s="132"/>
+      <c r="F47" s="132"/>
+      <c r="G47" s="132"/>
+      <c r="H47" s="132"/>
+      <c r="I47" s="132"/>
+      <c r="T47" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A48" s="134">
+        <v>6579489</v>
+      </c>
+      <c r="B48" s="85"/>
+      <c r="C48" s="85"/>
+      <c r="D48" s="85" t="s">
+        <v>178</v>
+      </c>
+      <c r="E48" s="85" t="s">
+        <v>178</v>
+      </c>
+      <c r="F48" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="G48" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="I48" s="115">
+        <v>12230</v>
+      </c>
+      <c r="J48" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="K48" s="85" t="s">
+        <v>60</v>
+      </c>
+      <c r="L48" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="M48" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="N48" s="122" t="s">
+        <v>53</v>
+      </c>
+      <c r="O48" s="115">
+        <v>100000000</v>
+      </c>
+      <c r="P48" s="85" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q48" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="R48" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="S48" s="123" t="b">
+        <v>1</v>
+      </c>
+      <c r="T48" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="U48" s="85" t="s">
+        <v>145</v>
+      </c>
+      <c r="V48" s="115">
+        <v>201480</v>
+      </c>
     </row>
     <row r="49" spans="1:1" ht="15.75" customHeight="1">
       <c r="A49" s="4"/>
@@ -10151,6 +10432,10 @@
       <c r="A986" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B47:I47"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10160,8 +10445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S981"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -10277,8 +10562,8 @@
       <c r="M2" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="56" t="s">
-        <v>54</v>
+      <c r="N2" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O2" s="60" t="s">
         <v>60</v>
@@ -10332,8 +10617,8 @@
       <c r="M3" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N3" s="56" t="s">
-        <v>54</v>
+      <c r="N3" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O3" s="60" t="s">
         <v>60</v>
@@ -10387,8 +10672,8 @@
       <c r="M4" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="56" t="s">
-        <v>54</v>
+      <c r="N4" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O4" s="60" t="s">
         <v>60</v>
@@ -10442,8 +10727,8 @@
       <c r="M5" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N5" s="56" t="s">
-        <v>54</v>
+      <c r="N5" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O5" s="60" t="s">
         <v>60</v>
@@ -10497,8 +10782,8 @@
       <c r="M6" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N6" s="56" t="s">
-        <v>54</v>
+      <c r="N6" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O6" s="60" t="s">
         <v>60</v>
@@ -10552,8 +10837,8 @@
       <c r="M7" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N7" s="56" t="s">
-        <v>54</v>
+      <c r="N7" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O7" s="60" t="s">
         <v>60</v>
@@ -10607,8 +10892,8 @@
       <c r="M8" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N8" s="56" t="s">
-        <v>54</v>
+      <c r="N8" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O8" s="60" t="s">
         <v>60</v>
@@ -10662,8 +10947,8 @@
       <c r="M9" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N9" s="56" t="s">
-        <v>54</v>
+      <c r="N9" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O9" s="60" t="s">
         <v>60</v>
@@ -10717,8 +11002,8 @@
       <c r="M10" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N10" s="56" t="s">
-        <v>54</v>
+      <c r="N10" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O10" s="60" t="s">
         <v>60</v>
@@ -10772,8 +11057,8 @@
       <c r="M11" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="N11" s="56" t="s">
-        <v>54</v>
+      <c r="N11" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O11" s="60" t="s">
         <v>60</v>
@@ -10827,8 +11112,8 @@
       <c r="M12" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="N12" s="37" t="s">
-        <v>54</v>
+      <c r="N12" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O12" s="66" t="s">
         <v>60</v>
@@ -10882,8 +11167,8 @@
       <c r="M13" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="N13" s="37" t="s">
-        <v>54</v>
+      <c r="N13" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O13" s="66" t="s">
         <v>60</v>
@@ -10937,8 +11222,8 @@
       <c r="M14" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="N14" s="37" t="s">
-        <v>54</v>
+      <c r="N14" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O14" s="66" t="s">
         <v>60</v>
@@ -10992,8 +11277,8 @@
       <c r="M15" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="N15" s="37" t="s">
-        <v>54</v>
+      <c r="N15" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O15" s="66" t="s">
         <v>60</v>
@@ -11047,8 +11332,8 @@
       <c r="M16" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="N16" s="37" t="s">
-        <v>54</v>
+      <c r="N16" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O16" s="66" t="s">
         <v>60</v>
@@ -11102,8 +11387,8 @@
       <c r="M17" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="N17" s="37" t="s">
-        <v>54</v>
+      <c r="N17" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O17" s="66" t="s">
         <v>60</v>
@@ -11157,8 +11442,8 @@
       <c r="M18" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="N18" s="37" t="s">
-        <v>54</v>
+      <c r="N18" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O18" s="66" t="s">
         <v>60</v>
@@ -11212,8 +11497,8 @@
       <c r="M19" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="N19" s="37" t="s">
-        <v>54</v>
+      <c r="N19" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O19" s="66" t="s">
         <v>60</v>
@@ -11267,8 +11552,8 @@
       <c r="M20" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="N20" s="37" t="s">
-        <v>54</v>
+      <c r="N20" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O20" s="66" t="s">
         <v>60</v>
@@ -11322,8 +11607,8 @@
       <c r="M21" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="N21" s="37" t="s">
-        <v>54</v>
+      <c r="N21" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O21" s="66" t="s">
         <v>60</v>
@@ -11378,7 +11663,7 @@
         <v>64</v>
       </c>
       <c r="N22" s="68" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="O22" s="74" t="s">
         <v>60</v>
@@ -11433,7 +11718,7 @@
         <v>64</v>
       </c>
       <c r="N23" s="68" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="O23" s="74" t="s">
         <v>60</v>
@@ -11488,7 +11773,7 @@
         <v>64</v>
       </c>
       <c r="N24" s="68" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="O24" s="74" t="s">
         <v>60</v>
@@ -11543,7 +11828,7 @@
         <v>64</v>
       </c>
       <c r="N25" s="68" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="O25" s="74" t="s">
         <v>60</v>
@@ -11598,7 +11883,7 @@
         <v>64</v>
       </c>
       <c r="N26" s="68" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="O26" s="74" t="s">
         <v>60</v>
@@ -11653,7 +11938,7 @@
         <v>64</v>
       </c>
       <c r="N27" s="68" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="O27" s="74" t="s">
         <v>60</v>
@@ -11708,7 +11993,7 @@
         <v>64</v>
       </c>
       <c r="N28" s="68" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="O28" s="74" t="s">
         <v>60</v>
@@ -11763,7 +12048,7 @@
         <v>64</v>
       </c>
       <c r="N29" s="68" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="O29" s="74" t="s">
         <v>60</v>
@@ -11818,7 +12103,7 @@
         <v>64</v>
       </c>
       <c r="N30" s="68" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="O30" s="74" t="s">
         <v>60</v>
@@ -11873,7 +12158,7 @@
         <v>64</v>
       </c>
       <c r="N31" s="68" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="O31" s="74" t="s">
         <v>60</v>
@@ -11894,10 +12179,25 @@
     <row r="32" spans="1:19" ht="15.75" customHeight="1">
       <c r="A32" s="82"/>
       <c r="G32" s="11"/>
-    </row>
-    <row r="33" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A33" s="11"/>
-      <c r="G33" s="11"/>
+      <c r="N32" s="68" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="136" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A33" s="135"/>
+      <c r="B33" s="138" t="s">
+        <v>179</v>
+      </c>
+      <c r="C33" s="138"/>
+      <c r="D33" s="138"/>
+      <c r="E33" s="138"/>
+      <c r="F33" s="138"/>
+      <c r="G33" s="138"/>
+      <c r="M33" s="135"/>
+      <c r="N33" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q33" s="128"/>
     </row>
     <row r="34" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A34" s="83">
@@ -11932,11 +12232,11 @@
       <c r="L34" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="M34" s="103" t="s">
+      <c r="M34" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="N34" s="85" t="s">
-        <v>54</v>
+      <c r="N34" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O34" s="85" t="s">
         <v>60</v>
@@ -11952,7 +12252,7 @@
       </c>
     </row>
     <row r="35" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A35" s="89">
+      <c r="A35" s="88">
         <v>6519013</v>
       </c>
       <c r="B35" s="85"/>
@@ -11984,11 +12284,11 @@
       <c r="L35" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="M35" s="103" t="s">
+      <c r="M35" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="N35" s="85" t="s">
-        <v>54</v>
+      <c r="N35" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O35" s="85" t="s">
         <v>60</v>
@@ -12004,30 +12304,30 @@
       </c>
     </row>
     <row r="36" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A36" s="90">
+      <c r="A36" s="89">
         <v>6596696</v>
       </c>
-      <c r="B36" s="104"/>
-      <c r="C36" s="104"/>
-      <c r="D36" s="91" t="s">
+      <c r="B36" s="102"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="E36" s="91" t="s">
+      <c r="E36" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="F36" s="91" t="s">
+      <c r="F36" s="90" t="s">
         <v>148</v>
       </c>
-      <c r="G36" s="91" t="s">
+      <c r="G36" s="90" t="s">
         <v>148</v>
       </c>
-      <c r="H36" s="105" t="s">
+      <c r="H36" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="I36" s="105" t="s">
+      <c r="I36" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="J36" s="105" t="s">
+      <c r="J36" s="103" t="s">
         <v>57</v>
       </c>
       <c r="K36" s="30" t="s">
@@ -12036,19 +12336,19 @@
       <c r="L36" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="M36" s="106" t="s">
+      <c r="M36" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="N36" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="O36" s="107" t="s">
+      <c r="N36" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="O36" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="P36" s="107" t="s">
+      <c r="P36" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="Q36" s="104" t="s">
+      <c r="Q36" s="102" t="s">
         <v>145</v>
       </c>
       <c r="R36" s="28">
@@ -12056,30 +12356,30 @@
       </c>
     </row>
     <row r="37" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A37" s="90">
+      <c r="A37" s="89">
         <v>6596733</v>
       </c>
-      <c r="B37" s="104"/>
-      <c r="C37" s="104"/>
-      <c r="D37" s="91" t="s">
+      <c r="B37" s="102"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="E37" s="91" t="s">
+      <c r="E37" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="F37" s="91" t="s">
+      <c r="F37" s="90" t="s">
         <v>150</v>
       </c>
-      <c r="G37" s="91" t="s">
+      <c r="G37" s="90" t="s">
         <v>150</v>
       </c>
-      <c r="H37" s="105" t="s">
+      <c r="H37" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="I37" s="105" t="s">
+      <c r="I37" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="J37" s="105" t="s">
+      <c r="J37" s="103" t="s">
         <v>57</v>
       </c>
       <c r="K37" s="30" t="s">
@@ -12088,19 +12388,19 @@
       <c r="L37" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="M37" s="106" t="s">
+      <c r="M37" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="N37" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="O37" s="107" t="s">
+      <c r="N37" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="O37" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="P37" s="107" t="s">
+      <c r="P37" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="Q37" s="104" t="s">
+      <c r="Q37" s="102" t="s">
         <v>145</v>
       </c>
       <c r="R37" s="28">
@@ -12108,27 +12408,29 @@
       </c>
     </row>
     <row r="38" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A38" s="108"/>
-      <c r="B38" s="109"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="110"/>
-      <c r="E38" s="110"/>
-      <c r="F38" s="110"/>
-      <c r="G38" s="110"/>
-      <c r="H38" s="111"/>
-      <c r="I38" s="111"/>
-      <c r="J38" s="111"/>
-      <c r="K38" s="112"/>
-      <c r="L38" s="112"/>
-      <c r="M38" s="113"/>
-      <c r="N38" s="110"/>
-      <c r="O38" s="114"/>
-      <c r="P38" s="114"/>
-      <c r="Q38" s="109"/>
-      <c r="R38" s="115"/>
+      <c r="A38" s="106"/>
+      <c r="B38" s="107"/>
+      <c r="C38" s="107"/>
+      <c r="D38" s="108"/>
+      <c r="E38" s="108"/>
+      <c r="F38" s="108"/>
+      <c r="G38" s="108"/>
+      <c r="H38" s="109"/>
+      <c r="I38" s="109"/>
+      <c r="J38" s="109"/>
+      <c r="K38" s="110"/>
+      <c r="L38" s="110"/>
+      <c r="M38" s="111"/>
+      <c r="N38" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="O38" s="112"/>
+      <c r="P38" s="112"/>
+      <c r="Q38" s="107"/>
+      <c r="R38" s="113"/>
     </row>
     <row r="39" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A39" s="116">
+      <c r="A39" s="114">
         <v>6596575</v>
       </c>
       <c r="B39" s="85"/>
@@ -12154,17 +12456,17 @@
       <c r="J39" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="K39" s="101" t="s">
+      <c r="K39" s="99" t="s">
         <v>95</v>
       </c>
       <c r="L39" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="M39" s="103" t="s">
+      <c r="M39" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="N39" s="85" t="s">
-        <v>54</v>
+      <c r="N39" s="68" t="s">
+        <v>173</v>
       </c>
       <c r="O39" s="85" t="s">
         <v>60</v>
@@ -12175,12 +12477,12 @@
       <c r="Q39" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="R39" s="117">
+      <c r="R39" s="115">
         <v>201534</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A40" s="116">
+      <c r="A40" s="114">
         <v>6596601</v>
       </c>
       <c r="B40" s="85"/>
@@ -12206,16 +12508,16 @@
       <c r="J40" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="K40" s="101" t="s">
+      <c r="K40" s="99" t="s">
         <v>95</v>
       </c>
       <c r="L40" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="M40" s="103" t="s">
+      <c r="M40" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="N40" s="85" t="s">
+      <c r="N40" s="141" t="s">
         <v>54</v>
       </c>
       <c r="O40" s="85" t="s">
@@ -12227,111 +12529,111 @@
       <c r="Q40" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="R40" s="117">
+      <c r="R40" s="115">
         <v>201534</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A41" s="116">
+      <c r="A41" s="114">
         <v>6596609</v>
       </c>
-      <c r="B41" s="104"/>
-      <c r="C41" s="104"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="102"/>
       <c r="D41" s="85" t="s">
         <v>152</v>
       </c>
       <c r="E41" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="F41" s="91" t="s">
+      <c r="F41" s="90" t="s">
         <v>157</v>
       </c>
-      <c r="G41" s="91" t="s">
+      <c r="G41" s="90" t="s">
         <v>157</v>
       </c>
-      <c r="H41" s="105" t="s">
+      <c r="H41" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="I41" s="105" t="s">
+      <c r="I41" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="J41" s="105" t="s">
+      <c r="J41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="K41" s="118" t="s">
+      <c r="K41" s="116" t="s">
         <v>95</v>
       </c>
       <c r="L41" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="M41" s="106" t="s">
+      <c r="M41" s="104" t="s">
         <v>64</v>
       </c>
       <c r="N41" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="O41" s="107" t="s">
+        <v>173</v>
+      </c>
+      <c r="O41" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="P41" s="107" t="s">
+      <c r="P41" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="Q41" s="104" t="s">
+      <c r="Q41" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="R41" s="119">
+      <c r="R41" s="117">
         <v>201534</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A42" s="116">
+      <c r="A42" s="114">
         <v>6596613</v>
       </c>
-      <c r="B42" s="104"/>
-      <c r="C42" s="104"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="102"/>
       <c r="D42" s="85" t="s">
         <v>152</v>
       </c>
       <c r="E42" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="F42" s="91" t="s">
+      <c r="F42" s="90" t="s">
         <v>159</v>
       </c>
-      <c r="G42" s="91" t="s">
+      <c r="G42" s="90" t="s">
         <v>159</v>
       </c>
-      <c r="H42" s="105" t="s">
+      <c r="H42" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="I42" s="105" t="s">
+      <c r="I42" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="105" t="s">
+      <c r="J42" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="K42" s="118" t="s">
+      <c r="K42" s="116" t="s">
         <v>95</v>
       </c>
       <c r="L42" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="M42" s="106" t="s">
+      <c r="M42" s="104" t="s">
         <v>64</v>
       </c>
       <c r="N42" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="O42" s="107" t="s">
+        <v>173</v>
+      </c>
+      <c r="O42" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="P42" s="107" t="s">
+      <c r="P42" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="Q42" s="104" t="s">
+      <c r="Q42" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="R42" s="119">
+      <c r="R42" s="117">
         <v>201534</v>
       </c>
     </row>
@@ -12342,16 +12644,18 @@
       <c r="D43" s="19"/>
       <c r="E43" s="18"/>
       <c r="F43" s="19"/>
-      <c r="G43" s="120"/>
-      <c r="H43" s="121"/>
-      <c r="I43" s="121"/>
-      <c r="J43" s="121"/>
-      <c r="K43" s="122"/>
-      <c r="L43" s="122"/>
-      <c r="M43" s="123"/>
-      <c r="N43" s="19"/>
-      <c r="O43" s="122"/>
-      <c r="P43" s="122"/>
+      <c r="G43" s="118"/>
+      <c r="H43" s="119"/>
+      <c r="I43" s="119"/>
+      <c r="J43" s="119"/>
+      <c r="K43" s="120"/>
+      <c r="L43" s="120"/>
+      <c r="M43" s="121"/>
+      <c r="N43" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="O43" s="120"/>
+      <c r="P43" s="120"/>
       <c r="Q43" s="18"/>
       <c r="R43" s="19"/>
     </row>
@@ -12382,17 +12686,17 @@
       <c r="J44" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="K44" s="101" t="s">
+      <c r="K44" s="99" t="s">
         <v>164</v>
       </c>
       <c r="L44" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="M44" s="103" t="s">
+      <c r="M44" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="N44" s="85" t="s">
-        <v>54</v>
+      <c r="N44" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="O44" s="85" t="s">
         <v>60</v>
@@ -12403,12 +12707,12 @@
       <c r="Q44" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="R44" s="102">
+      <c r="R44" s="100">
         <v>201536</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A45" s="89">
+      <c r="A45" s="88">
         <v>6596619</v>
       </c>
       <c r="B45" s="85"/>
@@ -12434,17 +12738,17 @@
       <c r="J45" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="K45" s="101" t="s">
+      <c r="K45" s="99" t="s">
         <v>164</v>
       </c>
       <c r="L45" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="M45" s="103" t="s">
+      <c r="M45" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="N45" s="85" t="s">
-        <v>54</v>
+      <c r="N45" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="O45" s="85" t="s">
         <v>60</v>
@@ -12455,179 +12759,242 @@
       <c r="Q45" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="R45" s="102">
+      <c r="R45" s="100">
         <v>201536</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A46" s="89">
+      <c r="A46" s="88">
         <v>6596630</v>
       </c>
-      <c r="B46" s="104"/>
-      <c r="C46" s="104"/>
+      <c r="B46" s="102"/>
+      <c r="C46" s="102"/>
       <c r="D46" s="85" t="s">
         <v>161</v>
       </c>
       <c r="E46" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="F46" s="91" t="s">
+      <c r="F46" s="90" t="s">
         <v>168</v>
       </c>
-      <c r="G46" s="91" t="s">
+      <c r="G46" s="90" t="s">
         <v>168</v>
       </c>
-      <c r="H46" s="105" t="s">
+      <c r="H46" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="I46" s="105" t="s">
+      <c r="I46" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="J46" s="105" t="s">
+      <c r="J46" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="K46" s="101" t="s">
+      <c r="K46" s="99" t="s">
         <v>164</v>
       </c>
       <c r="L46" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="M46" s="106" t="s">
+      <c r="M46" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="N46" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="O46" s="107" t="s">
+      <c r="N46" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="O46" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="P46" s="107" t="s">
+      <c r="P46" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="Q46" s="104" t="s">
+      <c r="Q46" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="R46" s="102">
+      <c r="R46" s="100">
         <v>201536</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A47" s="89">
+      <c r="A47" s="88">
         <v>6596686</v>
       </c>
-      <c r="B47" s="104"/>
-      <c r="C47" s="104"/>
+      <c r="B47" s="102"/>
+      <c r="C47" s="102"/>
       <c r="D47" s="85" t="s">
         <v>161</v>
       </c>
       <c r="E47" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="F47" s="91" t="s">
+      <c r="F47" s="90" t="s">
         <v>170</v>
       </c>
-      <c r="G47" s="91" t="s">
+      <c r="G47" s="90" t="s">
         <v>170</v>
       </c>
-      <c r="H47" s="105" t="s">
+      <c r="H47" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="I47" s="105" t="s">
+      <c r="I47" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="J47" s="105" t="s">
+      <c r="J47" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="K47" s="101" t="s">
+      <c r="K47" s="99" t="s">
         <v>164</v>
       </c>
       <c r="L47" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="M47" s="106" t="s">
+      <c r="M47" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="N47" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="O47" s="107" t="s">
+      <c r="N47" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="O47" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="P47" s="107" t="s">
+      <c r="P47" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="Q47" s="104" t="s">
+      <c r="Q47" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="R47" s="102">
+      <c r="R47" s="100">
         <v>201536</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="15.75" customHeight="1">
       <c r="A48" s="11"/>
       <c r="G48" s="11"/>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A49" s="11"/>
-      <c r="G49" s="11"/>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A50" s="11"/>
-      <c r="G50" s="11"/>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" customHeight="1">
+      <c r="N48" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" s="136" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A49" s="135"/>
+      <c r="B49" s="137" t="s">
+        <v>180</v>
+      </c>
+      <c r="C49" s="137"/>
+      <c r="D49" s="137"/>
+      <c r="E49" s="137"/>
+      <c r="F49" s="137"/>
+      <c r="G49" s="137"/>
+      <c r="M49" s="135"/>
+      <c r="N49" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q49" s="128"/>
+    </row>
+    <row r="50" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A50" s="134">
+        <v>6579489</v>
+      </c>
+      <c r="B50" s="85"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="85" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" s="85" t="s">
+        <v>178</v>
+      </c>
+      <c r="F50" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="G50" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="H50" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="J50" s="85" t="s">
+        <v>24</v>
+      </c>
+      <c r="K50" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="L50" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="M50" s="101" t="s">
+        <v>64</v>
+      </c>
+      <c r="N50" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="O50" s="85" t="s">
+        <v>60</v>
+      </c>
+      <c r="P50" s="85" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q50" s="85" t="s">
+        <v>145</v>
+      </c>
+      <c r="R50" s="28">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="15.75" customHeight="1">
       <c r="A51" s="11"/>
       <c r="G51" s="11"/>
     </row>
-    <row r="52" spans="1:7" ht="15.75" customHeight="1">
+    <row r="52" spans="1:18" ht="15.75" customHeight="1">
       <c r="A52" s="11"/>
       <c r="G52" s="11"/>
     </row>
-    <row r="53" spans="1:7" ht="15.75" customHeight="1">
+    <row r="53" spans="1:18" ht="15.75" customHeight="1">
       <c r="A53" s="11"/>
       <c r="G53" s="11"/>
     </row>
-    <row r="54" spans="1:7" ht="15.75" customHeight="1">
+    <row r="54" spans="1:18" ht="15.75" customHeight="1">
       <c r="A54" s="11"/>
       <c r="G54" s="11"/>
     </row>
-    <row r="55" spans="1:7" ht="15.75" customHeight="1">
+    <row r="55" spans="1:18" ht="15.75" customHeight="1">
       <c r="A55" s="11"/>
       <c r="G55" s="11"/>
     </row>
-    <row r="56" spans="1:7" ht="15.75" customHeight="1">
+    <row r="56" spans="1:18" ht="15.75" customHeight="1">
       <c r="A56" s="11"/>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="1:7" ht="15.75" customHeight="1">
+    <row r="57" spans="1:18" ht="15.75" customHeight="1">
       <c r="A57" s="11"/>
       <c r="G57" s="11"/>
     </row>
-    <row r="58" spans="1:7" ht="15.75" customHeight="1">
+    <row r="58" spans="1:18" ht="15.75" customHeight="1">
       <c r="A58" s="11"/>
       <c r="G58" s="11"/>
     </row>
-    <row r="59" spans="1:7" ht="15.75" customHeight="1">
+    <row r="59" spans="1:18" ht="15.75" customHeight="1">
       <c r="A59" s="11"/>
       <c r="G59" s="11"/>
     </row>
-    <row r="60" spans="1:7" ht="15.75" customHeight="1">
+    <row r="60" spans="1:18" ht="15.75" customHeight="1">
       <c r="A60" s="11"/>
       <c r="G60" s="11"/>
     </row>
-    <row r="61" spans="1:7" ht="15.75" customHeight="1">
+    <row r="61" spans="1:18" ht="15.75" customHeight="1">
       <c r="A61" s="11"/>
       <c r="G61" s="11"/>
     </row>
-    <row r="62" spans="1:7" ht="15.75" customHeight="1">
+    <row r="62" spans="1:18" ht="15.75" customHeight="1">
       <c r="A62" s="11"/>
       <c r="G62" s="11"/>
     </row>
-    <row r="63" spans="1:7" ht="15.75" customHeight="1">
+    <row r="63" spans="1:18" ht="15.75" customHeight="1">
       <c r="A63" s="11"/>
       <c r="G63" s="11"/>
     </row>
-    <row r="64" spans="1:7" ht="15.75" customHeight="1">
+    <row r="64" spans="1:18" ht="15.75" customHeight="1">
       <c r="A64" s="11"/>
       <c r="G64" s="11"/>
     </row>
@@ -16300,6 +16667,10 @@
       <c r="G981" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B49:G49"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -16309,8 +16680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD983"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -16408,8 +16779,8 @@
       <c r="G2" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="43" t="s">
-        <v>54</v>
+      <c r="H2" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I2" s="44">
         <v>1</v>
@@ -16448,8 +16819,8 @@
       <c r="G3" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="43" t="s">
-        <v>54</v>
+      <c r="H3" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I3" s="44">
         <v>1</v>
@@ -16488,8 +16859,8 @@
       <c r="G4" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="H4" s="43" t="s">
-        <v>54</v>
+      <c r="H4" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I4" s="44">
         <v>1</v>
@@ -16528,8 +16899,8 @@
       <c r="G5" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="H5" s="43" t="s">
-        <v>54</v>
+      <c r="H5" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I5" s="44">
         <v>1</v>
@@ -16568,8 +16939,8 @@
       <c r="G6" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="43" t="s">
-        <v>54</v>
+      <c r="H6" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I6" s="44">
         <v>1</v>
@@ -16608,8 +16979,8 @@
       <c r="G7" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="43" t="s">
-        <v>54</v>
+      <c r="H7" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I7" s="44">
         <v>1</v>
@@ -16648,8 +17019,8 @@
       <c r="G8" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="43" t="s">
-        <v>54</v>
+      <c r="H8" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I8" s="44">
         <v>1</v>
@@ -16688,8 +17059,8 @@
       <c r="G9" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="H9" s="43" t="s">
-        <v>54</v>
+      <c r="H9" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I9" s="44">
         <v>1</v>
@@ -16728,8 +17099,8 @@
       <c r="G10" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="43" t="s">
-        <v>54</v>
+      <c r="H10" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I10" s="44">
         <v>1</v>
@@ -16768,8 +17139,8 @@
       <c r="G11" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="43" t="s">
-        <v>54</v>
+      <c r="H11" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I11" s="44">
         <v>1</v>
@@ -16808,8 +17179,8 @@
       <c r="G12" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="36" t="s">
-        <v>54</v>
+      <c r="H12" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I12" s="47">
         <v>1</v>
@@ -16848,8 +17219,8 @@
       <c r="G13" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="H13" s="36" t="s">
-        <v>54</v>
+      <c r="H13" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I13" s="47">
         <v>1</v>
@@ -16888,8 +17259,8 @@
       <c r="G14" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="36" t="s">
-        <v>54</v>
+      <c r="H14" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I14" s="47">
         <v>1</v>
@@ -16928,8 +17299,8 @@
       <c r="G15" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="36" t="s">
-        <v>54</v>
+      <c r="H15" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I15" s="47">
         <v>1</v>
@@ -16968,8 +17339,8 @@
       <c r="G16" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="36" t="s">
-        <v>54</v>
+      <c r="H16" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I16" s="47">
         <v>1</v>
@@ -17008,8 +17379,8 @@
       <c r="G17" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="36" t="s">
-        <v>54</v>
+      <c r="H17" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I17" s="47">
         <v>1</v>
@@ -17048,8 +17419,8 @@
       <c r="G18" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="36" t="s">
-        <v>54</v>
+      <c r="H18" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I18" s="47">
         <v>1</v>
@@ -17088,8 +17459,8 @@
       <c r="G19" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="36" t="s">
-        <v>54</v>
+      <c r="H19" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I19" s="47">
         <v>1</v>
@@ -17128,8 +17499,8 @@
       <c r="G20" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="36" t="s">
-        <v>54</v>
+      <c r="H20" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I20" s="47">
         <v>1</v>
@@ -17168,8 +17539,8 @@
       <c r="G21" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="H21" s="36" t="s">
-        <v>54</v>
+      <c r="H21" s="51" t="s">
+        <v>173</v>
       </c>
       <c r="I21" s="47">
         <v>1</v>
@@ -17209,7 +17580,7 @@
         <v>104</v>
       </c>
       <c r="H22" s="51" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="I22" s="52">
         <v>1</v>
@@ -17249,7 +17620,7 @@
         <v>106</v>
       </c>
       <c r="H23" s="51" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="I23" s="52">
         <v>1</v>
@@ -17289,7 +17660,7 @@
         <v>104</v>
       </c>
       <c r="H24" s="51" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="I24" s="52">
         <v>1</v>
@@ -17329,7 +17700,7 @@
         <v>115</v>
       </c>
       <c r="H25" s="51" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="I25" s="52">
         <v>1</v>
@@ -17369,7 +17740,7 @@
         <v>110</v>
       </c>
       <c r="H26" s="51" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="I26" s="52">
         <v>1</v>
@@ -17409,7 +17780,7 @@
         <v>110</v>
       </c>
       <c r="H27" s="51" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="I27" s="52">
         <v>1</v>
@@ -17449,7 +17820,7 @@
         <v>113</v>
       </c>
       <c r="H28" s="51" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="I28" s="52">
         <v>1</v>
@@ -17489,7 +17860,7 @@
         <v>106</v>
       </c>
       <c r="H29" s="51" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="I29" s="52">
         <v>1</v>
@@ -17529,7 +17900,7 @@
         <v>110</v>
       </c>
       <c r="H30" s="51" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="I30" s="52">
         <v>1</v>
@@ -17569,7 +17940,7 @@
         <v>110</v>
       </c>
       <c r="H31" s="51" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="I31" s="52">
         <v>1</v>
@@ -17590,8 +17961,25 @@
         <v>201482</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H32" s="51" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="128" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B33" s="137" t="s">
+        <v>176</v>
+      </c>
+      <c r="C33" s="129"/>
+      <c r="D33" s="129"/>
+      <c r="E33" s="129"/>
+      <c r="F33" s="129"/>
+      <c r="G33" s="129"/>
+      <c r="H33" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="N33" s="136"/>
+    </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A34" s="83">
         <v>6519011</v>
@@ -17610,10 +17998,10 @@
       <c r="G34" s="84" t="s">
         <v>144</v>
       </c>
-      <c r="H34" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="I34" s="87">
+      <c r="H34" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I34" s="86">
         <v>1</v>
       </c>
       <c r="J34" s="30" t="s">
@@ -17622,7 +18010,7 @@
       <c r="K34" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="L34" s="88" t="s">
+      <c r="L34" s="87" t="s">
         <v>126</v>
       </c>
       <c r="M34" s="84" t="s">
@@ -17633,7 +18021,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A35" s="89">
+      <c r="A35" s="88">
         <v>6519013</v>
       </c>
       <c r="B35" s="84"/>
@@ -17650,10 +18038,10 @@
       <c r="G35" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="H35" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="I35" s="87">
+      <c r="H35" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I35" s="86">
         <v>1</v>
       </c>
       <c r="J35" s="30" t="s">
@@ -17662,7 +18050,7 @@
       <c r="K35" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="L35" s="88" t="s">
+      <c r="L35" s="87" t="s">
         <v>126</v>
       </c>
       <c r="M35" s="84" t="s">
@@ -17673,7 +18061,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A36" s="90">
+      <c r="A36" s="89">
         <v>6596696</v>
       </c>
       <c r="B36" s="84"/>
@@ -17684,16 +18072,16 @@
       <c r="E36" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="F36" s="91" t="s">
+      <c r="F36" s="90" t="s">
         <v>148</v>
       </c>
       <c r="G36" s="84" t="s">
         <v>149</v>
       </c>
-      <c r="H36" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="I36" s="87">
+      <c r="H36" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I36" s="86">
         <v>1</v>
       </c>
       <c r="J36" s="30" t="s">
@@ -17702,7 +18090,7 @@
       <c r="K36" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="L36" s="88" t="s">
+      <c r="L36" s="87" t="s">
         <v>126</v>
       </c>
       <c r="M36" s="84" t="s">
@@ -17713,7 +18101,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A37" s="90">
+      <c r="A37" s="89">
         <v>6596733</v>
       </c>
       <c r="B37" s="84"/>
@@ -17724,16 +18112,16 @@
       <c r="E37" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="F37" s="91" t="s">
+      <c r="F37" s="90" t="s">
         <v>150</v>
       </c>
       <c r="G37" s="84" t="s">
         <v>151</v>
       </c>
-      <c r="H37" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="I37" s="87">
+      <c r="H37" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I37" s="86">
         <v>1</v>
       </c>
       <c r="J37" s="30" t="s">
@@ -17742,7 +18130,7 @@
       <c r="K37" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="L37" s="88" t="s">
+      <c r="L37" s="87" t="s">
         <v>126</v>
       </c>
       <c r="M37" s="84" t="s">
@@ -17753,162 +18141,162 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A38" s="92">
+      <c r="A38" s="91">
         <v>6596575</v>
       </c>
-      <c r="B38" s="93"/>
-      <c r="C38" s="93"/>
-      <c r="D38" s="94" t="s">
+      <c r="B38" s="92"/>
+      <c r="C38" s="92"/>
+      <c r="D38" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="E38" s="94" t="s">
+      <c r="E38" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="F38" s="94" t="s">
+      <c r="F38" s="93" t="s">
         <v>153</v>
       </c>
-      <c r="G38" s="93" t="s">
+      <c r="G38" s="92" t="s">
         <v>154</v>
       </c>
-      <c r="H38" s="95" t="s">
+      <c r="H38" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I38" s="94">
+        <v>1</v>
+      </c>
+      <c r="J38" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="K38" s="96" t="s">
+        <v>96</v>
+      </c>
+      <c r="L38" s="97" t="s">
+        <v>126</v>
+      </c>
+      <c r="M38" s="92" t="s">
+        <v>145</v>
+      </c>
+      <c r="N38" s="98">
+        <v>201534</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A39" s="91">
+        <v>6596601</v>
+      </c>
+      <c r="B39" s="92"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="93" t="s">
+        <v>155</v>
+      </c>
+      <c r="G39" s="92" t="s">
+        <v>156</v>
+      </c>
+      <c r="H39" s="142" t="s">
         <v>54</v>
       </c>
-      <c r="I38" s="96">
+      <c r="I39" s="94">
         <v>1</v>
       </c>
-      <c r="J38" s="97" t="s">
+      <c r="J39" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="K38" s="98" t="s">
+      <c r="K39" s="96" t="s">
         <v>96</v>
       </c>
-      <c r="L38" s="99" t="s">
+      <c r="L39" s="97" t="s">
         <v>126</v>
       </c>
-      <c r="M38" s="93" t="s">
+      <c r="M39" s="92" t="s">
         <v>145</v>
       </c>
-      <c r="N38" s="100">
+      <c r="N39" s="98">
         <v>201534</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A39" s="92">
-        <v>6596601</v>
-      </c>
-      <c r="B39" s="93"/>
-      <c r="C39" s="93"/>
-      <c r="D39" s="94" t="s">
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A40" s="91">
+        <v>6596609</v>
+      </c>
+      <c r="B40" s="92"/>
+      <c r="C40" s="92"/>
+      <c r="D40" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="E39" s="94" t="s">
+      <c r="E40" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="F39" s="94" t="s">
-        <v>155</v>
-      </c>
-      <c r="G39" s="93" t="s">
-        <v>156</v>
-      </c>
-      <c r="H39" s="95" t="s">
-        <v>54</v>
-      </c>
-      <c r="I39" s="96">
+      <c r="F40" s="93" t="s">
+        <v>157</v>
+      </c>
+      <c r="G40" s="92" t="s">
+        <v>158</v>
+      </c>
+      <c r="H40" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I40" s="94">
         <v>1</v>
       </c>
-      <c r="J39" s="97" t="s">
+      <c r="J40" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="K39" s="98" t="s">
+      <c r="K40" s="96" t="s">
         <v>96</v>
       </c>
-      <c r="L39" s="99" t="s">
+      <c r="L40" s="97" t="s">
         <v>126</v>
       </c>
-      <c r="M39" s="93" t="s">
+      <c r="M40" s="92" t="s">
         <v>145</v>
       </c>
-      <c r="N39" s="100">
+      <c r="N40" s="98">
         <v>201534</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A40" s="92">
-        <v>6596609</v>
-      </c>
-      <c r="B40" s="93"/>
-      <c r="C40" s="93"/>
-      <c r="D40" s="94" t="s">
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A41" s="91">
+        <v>6596613</v>
+      </c>
+      <c r="B41" s="92"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="E40" s="94" t="s">
+      <c r="E41" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="F40" s="94" t="s">
-        <v>157</v>
-      </c>
-      <c r="G40" s="93" t="s">
-        <v>158</v>
-      </c>
-      <c r="H40" s="95" t="s">
-        <v>54</v>
-      </c>
-      <c r="I40" s="96">
+      <c r="F41" s="93" t="s">
+        <v>159</v>
+      </c>
+      <c r="G41" s="92" t="s">
+        <v>160</v>
+      </c>
+      <c r="H41" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="94">
         <v>1</v>
       </c>
-      <c r="J40" s="97" t="s">
+      <c r="J41" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="K40" s="98" t="s">
+      <c r="K41" s="96" t="s">
         <v>96</v>
       </c>
-      <c r="L40" s="99" t="s">
+      <c r="L41" s="97" t="s">
         <v>126</v>
       </c>
-      <c r="M40" s="93" t="s">
+      <c r="M41" s="92" t="s">
         <v>145</v>
       </c>
-      <c r="N40" s="100">
-        <v>201534</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A41" s="92">
-        <v>6596613</v>
-      </c>
-      <c r="B41" s="93"/>
-      <c r="C41" s="93"/>
-      <c r="D41" s="94" t="s">
-        <v>152</v>
-      </c>
-      <c r="E41" s="94" t="s">
-        <v>152</v>
-      </c>
-      <c r="F41" s="94" t="s">
-        <v>159</v>
-      </c>
-      <c r="G41" s="93" t="s">
-        <v>160</v>
-      </c>
-      <c r="H41" s="95" t="s">
-        <v>54</v>
-      </c>
-      <c r="I41" s="96">
-        <v>1</v>
-      </c>
-      <c r="J41" s="97" t="s">
-        <v>95</v>
-      </c>
-      <c r="K41" s="98" t="s">
-        <v>96</v>
-      </c>
-      <c r="L41" s="99" t="s">
-        <v>126</v>
-      </c>
-      <c r="M41" s="93" t="s">
-        <v>145</v>
-      </c>
-      <c r="N41" s="100">
+      <c r="N41" s="98">
         <v>201534</v>
       </c>
     </row>
@@ -17930,30 +18318,30 @@
       <c r="G42" s="84" t="s">
         <v>163</v>
       </c>
-      <c r="H42" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="I42" s="87">
+      <c r="H42" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I42" s="86">
         <v>1</v>
       </c>
-      <c r="J42" s="101" t="s">
+      <c r="J42" s="99" t="s">
         <v>164</v>
       </c>
       <c r="K42" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="L42" s="88" t="s">
+      <c r="L42" s="87" t="s">
         <v>126</v>
       </c>
       <c r="M42" s="84" t="s">
         <v>145</v>
       </c>
-      <c r="N42" s="102">
+      <c r="N42" s="100">
         <v>201536</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A43" s="89">
+      <c r="A43" s="88">
         <v>6596619</v>
       </c>
       <c r="B43" s="84"/>
@@ -17970,30 +18358,30 @@
       <c r="G43" s="84" t="s">
         <v>167</v>
       </c>
-      <c r="H43" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="I43" s="87">
+      <c r="H43" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I43" s="86">
         <v>1</v>
       </c>
-      <c r="J43" s="101" t="s">
+      <c r="J43" s="99" t="s">
         <v>164</v>
       </c>
       <c r="K43" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="L43" s="88" t="s">
+      <c r="L43" s="87" t="s">
         <v>126</v>
       </c>
       <c r="M43" s="84" t="s">
         <v>145</v>
       </c>
-      <c r="N43" s="102">
+      <c r="N43" s="100">
         <v>201536</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A44" s="89">
+      <c r="A44" s="88">
         <v>6596630</v>
       </c>
       <c r="B44" s="84"/>
@@ -18004,36 +18392,36 @@
       <c r="E44" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="F44" s="91" t="s">
+      <c r="F44" s="90" t="s">
         <v>168</v>
       </c>
       <c r="G44" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="H44" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="I44" s="87">
+      <c r="H44" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I44" s="86">
         <v>1</v>
       </c>
-      <c r="J44" s="101" t="s">
+      <c r="J44" s="99" t="s">
         <v>164</v>
       </c>
       <c r="K44" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="L44" s="88" t="s">
+      <c r="L44" s="87" t="s">
         <v>126</v>
       </c>
       <c r="M44" s="84" t="s">
         <v>145</v>
       </c>
-      <c r="N44" s="102">
+      <c r="N44" s="100">
         <v>201536</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A45" s="89">
+      <c r="A45" s="88">
         <v>6596686</v>
       </c>
       <c r="B45" s="84"/>
@@ -18044,37 +18432,93 @@
       <c r="E45" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="F45" s="91" t="s">
+      <c r="F45" s="90" t="s">
         <v>170</v>
       </c>
       <c r="G45" s="84" t="s">
         <v>171</v>
       </c>
-      <c r="H45" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="I45" s="87">
+      <c r="H45" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I45" s="86">
         <v>1</v>
       </c>
-      <c r="J45" s="101" t="s">
+      <c r="J45" s="99" t="s">
         <v>164</v>
       </c>
       <c r="K45" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="L45" s="88" t="s">
+      <c r="L45" s="87" t="s">
         <v>126</v>
       </c>
       <c r="M45" s="84" t="s">
         <v>145</v>
       </c>
-      <c r="N45" s="102">
+      <c r="N45" s="100">
         <v>201536</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H46" s="51" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" s="128" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B47" s="137" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="129"/>
+      <c r="D47" s="129"/>
+      <c r="E47" s="129"/>
+      <c r="F47" s="129"/>
+      <c r="G47" s="129"/>
+      <c r="H47" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="N47" s="136"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A48" s="134">
+        <v>6579489</v>
+      </c>
+      <c r="B48" s="84"/>
+      <c r="C48" s="84"/>
+      <c r="D48" s="85" t="s">
+        <v>178</v>
+      </c>
+      <c r="E48" s="85" t="s">
+        <v>178</v>
+      </c>
+      <c r="F48" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="G48" s="84" t="s">
+        <v>182</v>
+      </c>
+      <c r="H48" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="I48" s="86">
+        <v>1</v>
+      </c>
+      <c r="J48" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K48" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="L48" s="87" t="s">
+        <v>126</v>
+      </c>
+      <c r="M48" s="84" t="s">
+        <v>145</v>
+      </c>
+      <c r="N48" s="28">
+        <v>201480</v>
+      </c>
+    </row>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -19011,6 +19455,10 @@
     <row r="982" ht="15.75" customHeight="1"/>
     <row r="983" ht="15.75" customHeight="1"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B47:G47"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
RPR Fiscal Year Issue Partially Fix
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asif/Documents/AMT-TestFrameWork/src/main/resources/dataCreate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56041F8A-353C-5F42-BA31-AC0C07D398B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF4E16D-91D9-3F47-A2B7-B957522F9E52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2660" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="115">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -182,9 +182,6 @@
     <t>QA Testing</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>startDate</t>
   </si>
   <si>
@@ -319,12 +316,72 @@
   <si>
     <t>Space66280601</t>
   </si>
+  <si>
+    <t>EditRevisionProperty01</t>
+  </si>
+  <si>
+    <t>ERLease1</t>
+  </si>
+  <si>
+    <t>01/01/2016</t>
+  </si>
+  <si>
+    <t>ERLease1Space</t>
+  </si>
+  <si>
+    <t>Lease Year</t>
+  </si>
+  <si>
+    <t>ERLease2</t>
+  </si>
+  <si>
+    <t>ERLease2Space</t>
+  </si>
+  <si>
+    <t>LIn6628070</t>
+  </si>
+  <si>
+    <t>LIn6628070Sp</t>
+  </si>
+  <si>
+    <t>LIn6628072</t>
+  </si>
+  <si>
+    <t>LIn6628072Sp</t>
+  </si>
+  <si>
+    <t>LIn6628073</t>
+  </si>
+  <si>
+    <t>LIn6628073Sp</t>
+  </si>
+  <si>
+    <t>LIn6628074</t>
+  </si>
+  <si>
+    <t>LIn6628074Sp</t>
+  </si>
+  <si>
+    <t>LIn6628075</t>
+  </si>
+  <si>
+    <t>LIn6628075Sp</t>
+  </si>
+  <si>
+    <t>LIn6628076</t>
+  </si>
+  <si>
+    <t>LIn6628076Sp</t>
+  </si>
+  <si>
+    <t>One Time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -382,8 +439,15 @@
       <name val="Consolas"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,14 +462,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -474,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -525,30 +601,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -557,13 +615,92 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -883,19 +1020,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V956"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="I1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
     <col min="8" max="8" width="8.83203125" customWidth="1"/>
     <col min="9" max="9" width="8.5" customWidth="1"/>
     <col min="10" max="10" width="9.6640625" customWidth="1"/>
@@ -960,13 +1097,13 @@
         <v>12</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>13</v>
@@ -975,288 +1112,760 @@
         <v>14</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
+        <v>6545928</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="26">
+        <v>12230</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
-        <v>6545928</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="7">
-        <v>12230</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="26" t="s">
         <v>31</v>
       </c>
       <c r="N2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="26">
         <v>100000000</v>
       </c>
-      <c r="P2" s="7" t="s">
-        <v>81</v>
+      <c r="P2" s="26" t="s">
+        <v>80</v>
       </c>
       <c r="Q2" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="R2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="S2" s="7" t="b">
+      <c r="S2" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="T2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="V2" s="16">
+      <c r="T2" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" s="28">
         <v>201480</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24">
+    <row r="3" spans="1:22" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="30">
         <v>6628089</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="17" t="s">
+      <c r="D3" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="29">
         <v>12230</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="29">
+        <v>100000000</v>
+      </c>
+      <c r="P3" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="Q3" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U3" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="V3" s="33">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="26">
+        <v>12230</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="17">
-        <v>100000000</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q3" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="R3" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="S3" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="T3" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="U3" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="V3" s="32">
-        <v>201480</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="7">
-        <v>12230</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="26" t="s">
         <v>31</v>
       </c>
       <c r="N4" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="26">
         <v>100000000</v>
       </c>
-      <c r="P4" s="7" t="s">
-        <v>81</v>
+      <c r="P4" s="26" t="s">
+        <v>80</v>
       </c>
       <c r="Q4" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="S4" s="7" t="b">
+      <c r="S4" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="T4" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="V4" s="16">
+      <c r="T4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U4" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="V4" s="28">
         <v>201480</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
+    <row r="5" spans="1:22" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="28">
         <v>6628060</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="17" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="29">
         <v>12230</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="29">
+        <v>100000000</v>
+      </c>
+      <c r="P5" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="Q5" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="S5" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U5" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5" s="33">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="28">
+        <v>6628061</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="29">
+        <v>12230</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M6" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="30" t="s">
+      <c r="N6" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="O5" s="17">
+      <c r="O6" s="29">
         <v>100000000</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P6" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q6" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="Q5" s="30" t="s">
+      <c r="R6" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="R5" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="S5" s="17" t="b">
+      <c r="S6" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="T5" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="U5" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="V5" s="32">
+      <c r="T6" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U6" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="V6" s="33">
         <v>201480</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+    <row r="7" spans="1:22" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28">
+        <v>6628062</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="29">
+        <v>12230</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" s="29">
+        <v>100000000</v>
+      </c>
+      <c r="P7" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q7" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="R7" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="S7" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U7" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="V7" s="33">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="41">
+        <v>6628070</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="37">
+        <v>12230</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" s="37">
+        <v>100000000</v>
+      </c>
+      <c r="P8" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="R8" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="S8" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U8" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="V8" s="33">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="41">
+        <v>6628072</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="37">
+        <v>12230</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" s="37">
+        <v>100000000</v>
+      </c>
+      <c r="P9" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q9" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="R9" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="S9" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U9" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="V9" s="33">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="41">
+        <v>6628073</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="37">
+        <v>12230</v>
+      </c>
+      <c r="J10" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" s="37">
+        <v>100000000</v>
+      </c>
+      <c r="P10" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q10" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="R10" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="S10" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U10" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10" s="33">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="41">
+        <v>6628074</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="37">
+        <v>12230</v>
+      </c>
+      <c r="J11" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" s="37">
+        <v>100000000</v>
+      </c>
+      <c r="P11" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q11" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="R11" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="S11" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U11" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="V11" s="33">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="41">
+        <v>6628075</v>
+      </c>
+      <c r="C12" s="40"/>
+      <c r="D12" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="37">
+        <v>12230</v>
+      </c>
+      <c r="J12" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" s="37">
+        <v>100000000</v>
+      </c>
+      <c r="P12" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q12" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="R12" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="S12" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U12" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="V12" s="33">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="41">
+        <v>6628076</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="37">
+        <v>12230</v>
+      </c>
+      <c r="J13" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="O13" s="37">
+        <v>100000000</v>
+      </c>
+      <c r="P13" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q13" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="R13" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="S13" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U13" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13" s="33">
+        <v>201480</v>
+      </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
@@ -4098,27 +4707,27 @@
   <dimension ref="A1:R950"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="19" style="10" customWidth="1"/>
-    <col min="4" max="4" width="29.5" style="10" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="29.5" style="10" customWidth="1"/>
-    <col min="7" max="7" width="28.5" style="10" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="7" customWidth="1"/>
-    <col min="9" max="10" width="14.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="20" style="10" customWidth="1"/>
+    <col min="8" max="8" width="12" style="7" customWidth="1"/>
+    <col min="9" max="10" width="11" style="7" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" style="10" customWidth="1"/>
     <col min="12" max="12" width="14.5" style="10" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" style="12" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="14.5" style="7"/>
-    <col min="16" max="16" width="20.6640625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" style="18" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" style="12" customWidth="1"/>
+    <col min="14" max="14" width="12" style="7" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" style="18" customWidth="1"/>
     <col min="18" max="18" width="9.1640625" style="7" customWidth="1"/>
     <col min="19" max="16384" width="14.5" style="10"/>
   </cols>
@@ -4161,7 +4770,7 @@
         <v>21</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>14</v>
@@ -4173,243 +4782,611 @@
         <v>44</v>
       </c>
       <c r="Q1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="28">
+        <v>6628089</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O2" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16">
-        <v>6628089</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="20" t="s">
+      <c r="P2" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" s="26">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26">
+        <v>6545928</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="21" t="s">
+      <c r="J3" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L3" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="20" t="s">
+      <c r="M3" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" s="26">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O4" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" s="26">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="28">
+        <v>6628060</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="P2" s="21" t="s">
+      <c r="K5" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O5" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="R2" s="20">
+      <c r="Q5" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="R5" s="26">
         <v>201480</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>6545928</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="20" t="s">
+    <row r="6" spans="1:18" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="28">
+        <v>6628061</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I6" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="21" t="s">
+      <c r="J6" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="N3" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="O3" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="P3" s="21" t="s">
+      <c r="M6" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O6" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="R3" s="20">
+      <c r="Q6" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" s="49">
         <v>201480</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+    <row r="7" spans="1:18" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28">
+        <v>6628062</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="20" t="s">
+      <c r="O7" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="P7" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q7" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" s="49">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="41">
+        <v>6628070</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I8" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="21" t="s">
+      <c r="J8" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" s="21" t="s">
+      <c r="M8" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="N8" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O8" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="P8" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="R4" s="20">
+      <c r="Q8" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="R8" s="43">
         <v>201480</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
-        <v>6628060</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H5" s="20" t="s">
+    <row r="9" spans="1:18" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="41">
+        <v>6628072</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I9" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K5" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="21" t="s">
+      <c r="J9" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="O5" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="P5" s="21" t="s">
+      <c r="M9" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O9" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="Q5" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="R5" s="20">
+      <c r="Q9" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="R9" s="43">
         <v>201480</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="G13" s="11"/>
+    <row r="10" spans="1:18" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="41">
+        <v>6628073</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O10" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="R10" s="43">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="41">
+        <v>6628074</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O11" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="P11" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q11" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="R11" s="43">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="41">
+        <v>6628075</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="M12" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O12" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="P12" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q12" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="R12" s="43">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="41">
+        <v>6628076</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="N13" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="O13" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="P13" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q13" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="R13" s="43">
+        <v>201480</v>
+      </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
@@ -8169,19 +9146,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N952"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="29.5" style="10" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="31.83203125" customWidth="1"/>
-    <col min="7" max="7" width="43.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="22" style="10" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" style="2" customWidth="1"/>
     <col min="10" max="11" width="12.33203125" customWidth="1"/>
@@ -8220,56 +9197,56 @@
         <v>27</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="29" t="s">
-        <v>66</v>
+      <c r="L1" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16">
         <v>6628089</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>61</v>
+      <c r="D2" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>91</v>
+      <c r="H2" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="I2" s="17">
         <v>1</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="M2" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" s="20">
+      <c r="N2" s="19">
         <v>201480</v>
       </c>
     </row>
@@ -8280,24 +9257,24 @@
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>89</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I3" s="7">
         <v>1</v>
       </c>
-      <c r="J3" s="28">
+      <c r="J3" s="22">
         <v>42736</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -8307,7 +9284,7 @@
         <v>123</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N3" s="7">
         <v>201480</v>
@@ -8315,27 +9292,27 @@
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="I4" s="7">
         <v>1</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="22">
         <v>42736</v>
       </c>
       <c r="K4" s="7" t="s">
@@ -8345,7 +9322,7 @@
         <v>123</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N4" s="7">
         <v>201480</v>
@@ -8356,25 +9333,25 @@
         <v>6628060</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="I5" s="7">
         <v>1</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="22">
         <v>42736</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -8384,22 +9361,316 @@
         <v>123</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N5" s="7">
         <v>201480</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
+        <v>6628061</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" s="19">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16">
+        <v>6628062</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="19">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="41">
+        <v>6628070</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="19">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="41">
+        <v>6628072</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" s="19">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="41">
+        <v>6628073</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="7">
+        <v>1</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10" s="19">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="41">
+        <v>6628074</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="7">
+        <v>1</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N11" s="19">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="41">
+        <v>6628075</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="7">
+        <v>1</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N12" s="19">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="41">
+        <v>6628076</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="7">
+        <v>1</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13" s="19">
+        <v>201480</v>
+      </c>
+    </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9347,20 +10618,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB958"/>
+  <dimension ref="A1:AB956"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
-    <col min="5" max="5" width="33.1640625" customWidth="1"/>
-    <col min="6" max="7" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
     <col min="9" max="9" width="17.83203125" customWidth="1"/>
     <col min="10" max="10" width="21.33203125" customWidth="1"/>
@@ -9369,7 +10641,7 @@
     <col min="13" max="14" width="14.5" customWidth="1"/>
     <col min="15" max="15" width="8.6640625" customWidth="1"/>
     <col min="16" max="16" width="16.5" customWidth="1"/>
-    <col min="17" max="17" width="18.5" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" customWidth="1"/>
     <col min="18" max="28" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9393,7 +10665,7 @@
         <v>33</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>34</v>
@@ -9408,7 +10680,7 @@
         <v>37</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>38</v>
@@ -9423,10 +10695,10 @@
         <v>14</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
@@ -9439,244 +10711,611 @@
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
     </row>
-    <row r="2" spans="1:28" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16">
+    <row r="2" spans="1:28" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="28">
         <v>6628089</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="25" t="s">
+      <c r="I2" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" s="29">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26">
+        <v>6545928</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="26"/>
+      <c r="M3" s="55">
+        <v>42736</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="26">
+        <v>1254</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q3" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" s="26">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="26"/>
+      <c r="M4" s="55">
+        <v>42736</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="26">
+        <v>1254</v>
+      </c>
+      <c r="P4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q4" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" s="26">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="28">
+        <v>6628060</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="G5" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O5" s="26">
+        <v>1254</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="R5" s="26">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="28">
+        <v>6628061</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="K6" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="M6" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O6" s="26">
+        <v>1254</v>
+      </c>
+      <c r="P6" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" s="26">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28">
+        <v>6628062</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J7" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O7" s="26">
+        <v>1254</v>
+      </c>
+      <c r="P7" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" s="26">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="41">
+        <v>6628070</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="M8" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8" s="39">
+        <v>1254</v>
+      </c>
+      <c r="P8" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q8" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="R8" s="39">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="41">
+        <v>6628072</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="M9" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9" s="39">
+        <v>1254</v>
+      </c>
+      <c r="P9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q9" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="R9" s="39">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="41">
+        <v>6628073</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="L10" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M10" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="N10" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="R2" s="17">
+      <c r="O10" s="39">
+        <v>1254</v>
+      </c>
+      <c r="P10" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q10" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="R10" s="39">
         <v>201480</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>6545928</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I3" s="7" t="s">
+    <row r="11" spans="1:28" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="41">
+        <v>6628074</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="I11" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J11" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="28">
-        <v>42736</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="7">
+      <c r="M11" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="N11" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" s="39">
         <v>1254</v>
       </c>
-      <c r="P3" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="R3" s="7">
+      <c r="P11" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="R11" s="39">
         <v>201480</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+    <row r="12" spans="1:28" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="41">
+        <v>6628075</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="M12" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="O12" s="39">
+        <v>1254</v>
+      </c>
+      <c r="P12" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="Q12" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="R12" s="39">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="41">
+        <v>6628076</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="28">
-        <v>42736</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="7">
+      <c r="J13" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="L13" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="M13" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="39">
         <v>1254</v>
       </c>
-      <c r="P4" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="R4" s="7">
+      <c r="P13" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q13" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="R13" s="39">
         <v>201480</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
-        <v>6628060</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="N5" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="O5" s="7">
-        <v>1254</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="R5" s="7">
-        <v>201480</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10601,8 +12240,6 @@
     <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Schedule Table Method Update
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asif/Documents/AMT-TestFrameWork/src/main/resources/dataCreate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D041691-3AD9-484A-B0A2-B4D77887B166}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D7449E-C005-3948-BF41-289ED50CC717}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2660" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="RecurringPayment" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="150">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -418,12 +419,75 @@
   <si>
     <t>Yes</t>
   </si>
+  <si>
+    <t>Lin6628084</t>
+  </si>
+  <si>
+    <t>Lin6628085</t>
+  </si>
+  <si>
+    <t>Lin6628087</t>
+  </si>
+  <si>
+    <t>Lin6628088</t>
+  </si>
+  <si>
+    <t>Lin6628090</t>
+  </si>
+  <si>
+    <t>Lin6628091</t>
+  </si>
+  <si>
+    <t>Lin6628071</t>
+  </si>
+  <si>
+    <t>Lin6628092</t>
+  </si>
+  <si>
+    <t>Lin6628094</t>
+  </si>
+  <si>
+    <t>Lin6628095</t>
+  </si>
+  <si>
+    <t>Lin6628084Sp</t>
+  </si>
+  <si>
+    <t>Lin6628085Sp</t>
+  </si>
+  <si>
+    <t>Lin6628087Sp</t>
+  </si>
+  <si>
+    <t>Lin6628088Sp</t>
+  </si>
+  <si>
+    <t>Lin6628090Sp</t>
+  </si>
+  <si>
+    <t>Lin6628091Sp</t>
+  </si>
+  <si>
+    <t>Lin6628071Sp</t>
+  </si>
+  <si>
+    <t>Lin6628092Sp</t>
+  </si>
+  <si>
+    <t>Lin6628094Sp</t>
+  </si>
+  <si>
+    <t>Lin6628095Sp</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -488,8 +552,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,6 +599,24 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -598,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -752,6 +839,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1069,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V956"/>
+  <dimension ref="A1:V954"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1971,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="T14" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="U14" s="32" t="s">
         <v>67</v>
@@ -2033,7 +2155,7 @@
         <v>1</v>
       </c>
       <c r="T15" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="U15" s="32" t="s">
         <v>67</v>
@@ -2095,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="T16" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="U16" s="32" t="s">
         <v>67</v>
@@ -2157,7 +2279,7 @@
         <v>1</v>
       </c>
       <c r="T17" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="U17" s="32" t="s">
         <v>67</v>
@@ -2219,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="T18" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="U18" s="32" t="s">
         <v>67</v>
@@ -2281,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="T19" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="U19" s="32" t="s">
         <v>67</v>
@@ -2291,34 +2413,644 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
+      <c r="A20" s="57">
+        <v>6628084</v>
+      </c>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="58">
+        <v>12230</v>
+      </c>
+      <c r="J20" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L20" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="O20" s="58">
+        <v>100000000</v>
+      </c>
+      <c r="P20" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q20" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="R20" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="S20" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T20" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U20" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="V20" s="68">
+        <v>201480</v>
+      </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
+      <c r="A21" s="57">
+        <v>6628085</v>
+      </c>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="58">
+        <v>12230</v>
+      </c>
+      <c r="J21" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="O21" s="58">
+        <v>100000000</v>
+      </c>
+      <c r="P21" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q21" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="R21" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="S21" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T21" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U21" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="V21" s="68">
+        <v>201480</v>
+      </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
+      <c r="A22" s="57">
+        <v>6628087</v>
+      </c>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="58">
+        <v>12230</v>
+      </c>
+      <c r="J22" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L22" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N22" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="O22" s="58">
+        <v>100000000</v>
+      </c>
+      <c r="P22" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q22" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="R22" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="S22" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T22" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U22" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="V22" s="68">
+        <v>201480</v>
+      </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
+      <c r="A23" s="57">
+        <v>6628088</v>
+      </c>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="58">
+        <v>12230</v>
+      </c>
+      <c r="J23" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K23" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L23" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N23" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="O23" s="58">
+        <v>100000000</v>
+      </c>
+      <c r="P23" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q23" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="R23" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="S23" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T23" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U23" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="V23" s="68">
+        <v>201480</v>
+      </c>
     </row>
     <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
+      <c r="A24" s="57">
+        <v>6628090</v>
+      </c>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="58">
+        <v>12230</v>
+      </c>
+      <c r="J24" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L24" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N24" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="O24" s="58">
+        <v>100000000</v>
+      </c>
+      <c r="P24" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q24" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="R24" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="S24" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T24" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U24" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="V24" s="68">
+        <v>201480</v>
+      </c>
     </row>
     <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
+      <c r="A25" s="57">
+        <v>6628091</v>
+      </c>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="58">
+        <v>12230</v>
+      </c>
+      <c r="J25" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="M25" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N25" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="O25" s="58">
+        <v>100000000</v>
+      </c>
+      <c r="P25" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q25" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="R25" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="S25" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T25" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U25" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="V25" s="68">
+        <v>201480</v>
+      </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
+      <c r="A26" s="57">
+        <v>6628071</v>
+      </c>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="58">
+        <v>12230</v>
+      </c>
+      <c r="J26" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="M26" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N26" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="O26" s="58">
+        <v>100000000</v>
+      </c>
+      <c r="P26" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q26" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="R26" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="S26" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T26" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U26" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="V26" s="68">
+        <v>201480</v>
+      </c>
     </row>
     <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
+      <c r="A27" s="57">
+        <v>6628092</v>
+      </c>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="58">
+        <v>12230</v>
+      </c>
+      <c r="J27" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N27" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="O27" s="58">
+        <v>100000000</v>
+      </c>
+      <c r="P27" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q27" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="R27" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="S27" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T27" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U27" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="V27" s="68">
+        <v>201480</v>
+      </c>
     </row>
     <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
+      <c r="A28" s="57">
+        <v>6628094</v>
+      </c>
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="58">
+        <v>12230</v>
+      </c>
+      <c r="J28" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L28" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N28" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="O28" s="58">
+        <v>100000000</v>
+      </c>
+      <c r="P28" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q28" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="R28" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="S28" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T28" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U28" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="V28" s="68">
+        <v>201480</v>
+      </c>
     </row>
     <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="A29" s="57">
+        <v>6628095</v>
+      </c>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="58">
+        <v>12230</v>
+      </c>
+      <c r="J29" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L29" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="M29" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N29" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="O29" s="58">
+        <v>100000000</v>
+      </c>
+      <c r="P29" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q29" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="R29" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="S29" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T29" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="U29" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="V29" s="68">
+        <v>201480</v>
+      </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
@@ -5095,13 +5827,8 @@
     <row r="954" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A954" s="4"/>
     </row>
-    <row r="955" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A955" s="4"/>
-    </row>
-    <row r="956" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A956" s="4"/>
-    </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5109,10 +5836,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R950"/>
+  <dimension ref="A1:R948"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5120,10 +5847,10 @@
     <col min="1" max="1" width="10.5" style="10" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" style="10" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="20" style="10" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" style="10" customWidth="1"/>
     <col min="8" max="8" width="12" style="7" customWidth="1"/>
     <col min="9" max="10" width="11" style="7" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" style="10" customWidth="1"/>
@@ -5828,7 +6555,7 @@
         <v>57</v>
       </c>
       <c r="N14" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="O14" s="50" t="s">
         <v>53</v>
@@ -5878,7 +6605,7 @@
         <v>57</v>
       </c>
       <c r="N15" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="O15" s="50" t="s">
         <v>53</v>
@@ -5928,7 +6655,7 @@
         <v>57</v>
       </c>
       <c r="N16" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="O16" s="50" t="s">
         <v>53</v>
@@ -5978,7 +6705,7 @@
         <v>57</v>
       </c>
       <c r="N17" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="O17" s="50" t="s">
         <v>53</v>
@@ -6028,7 +6755,7 @@
         <v>57</v>
       </c>
       <c r="N18" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="O18" s="50" t="s">
         <v>53</v>
@@ -6078,7 +6805,7 @@
         <v>57</v>
       </c>
       <c r="N19" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="O19" s="50" t="s">
         <v>53</v>
@@ -6094,44 +6821,544 @@
       </c>
     </row>
     <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="A20" s="57">
+        <v>6628084</v>
+      </c>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="61" t="str">
+        <f>CONCATENATE("Lin",A20)</f>
+        <v>Lin6628084</v>
+      </c>
+      <c r="G20" s="61" t="str">
+        <f>CONCATENATE("Lin",A20)</f>
+        <v>Lin6628084</v>
+      </c>
+      <c r="H20" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="L20" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="O20" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="P20" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q20" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R20" s="63">
+        <v>201480</v>
+      </c>
     </row>
     <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="A21" s="57">
+        <v>6628085</v>
+      </c>
+      <c r="B21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="61" t="str">
+        <f>CONCATENATE("Lin",A21)</f>
+        <v>Lin6628085</v>
+      </c>
+      <c r="G21" s="61" t="str">
+        <f>CONCATENATE("Lin",A21)</f>
+        <v>Lin6628085</v>
+      </c>
+      <c r="H21" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="L21" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="N21" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="O21" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="P21" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q21" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R21" s="63">
+        <v>201480</v>
+      </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="A22" s="57">
+        <v>6628087</v>
+      </c>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="61" t="str">
+        <f>CONCATENATE("Lin",A22)</f>
+        <v>Lin6628087</v>
+      </c>
+      <c r="G22" s="61" t="str">
+        <f>CONCATENATE("Lin",A22)</f>
+        <v>Lin6628087</v>
+      </c>
+      <c r="H22" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="K22" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="L22" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="N22" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="O22" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="P22" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q22" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R22" s="63">
+        <v>201480</v>
+      </c>
     </row>
     <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="G23" s="11"/>
+      <c r="A23" s="57">
+        <v>6628088</v>
+      </c>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="61" t="str">
+        <f>CONCATENATE("Lin",A23)</f>
+        <v>Lin6628088</v>
+      </c>
+      <c r="G23" s="61" t="str">
+        <f>CONCATENATE("Lin",A23)</f>
+        <v>Lin6628088</v>
+      </c>
+      <c r="H23" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="L23" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="N23" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="O23" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="P23" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q23" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R23" s="63">
+        <v>201480</v>
+      </c>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="G24" s="11"/>
+      <c r="A24" s="57">
+        <v>6628090</v>
+      </c>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="61" t="str">
+        <f>CONCATENATE("Lin",A24)</f>
+        <v>Lin6628090</v>
+      </c>
+      <c r="G24" s="61" t="str">
+        <f>CONCATENATE("Lin",A24)</f>
+        <v>Lin6628090</v>
+      </c>
+      <c r="H24" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="L24" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="M24" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="N24" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="O24" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="P24" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q24" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R24" s="63">
+        <v>201480</v>
+      </c>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="G25" s="11"/>
+      <c r="A25" s="57">
+        <v>6628091</v>
+      </c>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="61" t="str">
+        <f>CONCATENATE("Lin",A25)</f>
+        <v>Lin6628091</v>
+      </c>
+      <c r="G25" s="61" t="str">
+        <f>CONCATENATE("Lin",A25)</f>
+        <v>Lin6628091</v>
+      </c>
+      <c r="H25" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="K25" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="L25" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="M25" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="N25" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="O25" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="P25" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q25" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R25" s="63">
+        <v>201480</v>
+      </c>
     </row>
     <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="A26" s="57">
+        <v>6628071</v>
+      </c>
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="61" t="str">
+        <f>CONCATENATE("Lin",A26)</f>
+        <v>Lin6628071</v>
+      </c>
+      <c r="G26" s="61" t="str">
+        <f>CONCATENATE("Lin",A26)</f>
+        <v>Lin6628071</v>
+      </c>
+      <c r="H26" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="K26" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="L26" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="N26" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="O26" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="P26" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q26" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R26" s="63">
+        <v>201480</v>
+      </c>
     </row>
     <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="G27" s="11"/>
+      <c r="A27" s="57">
+        <v>6628092</v>
+      </c>
+      <c r="B27" s="62"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="61" t="str">
+        <f>CONCATENATE("Lin",A27)</f>
+        <v>Lin6628092</v>
+      </c>
+      <c r="G27" s="61" t="str">
+        <f>CONCATENATE("Lin",A27)</f>
+        <v>Lin6628092</v>
+      </c>
+      <c r="H27" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="L27" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="M27" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="N27" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="O27" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="P27" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q27" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R27" s="63">
+        <v>201480</v>
+      </c>
     </row>
     <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="G28" s="11"/>
+      <c r="A28" s="57">
+        <v>6628094</v>
+      </c>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="61" t="str">
+        <f>CONCATENATE("Lin",A28)</f>
+        <v>Lin6628094</v>
+      </c>
+      <c r="G28" s="61" t="str">
+        <f>CONCATENATE("Lin",A28)</f>
+        <v>Lin6628094</v>
+      </c>
+      <c r="H28" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="K28" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="L28" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="M28" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="N28" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="O28" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="P28" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q28" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R28" s="63">
+        <v>201480</v>
+      </c>
     </row>
     <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="A29" s="57">
+        <v>6628095</v>
+      </c>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="61" t="str">
+        <f>CONCATENATE("Lin",A29)</f>
+        <v>Lin6628095</v>
+      </c>
+      <c r="G29" s="61" t="str">
+        <f>CONCATENATE("Lin",A29)</f>
+        <v>Lin6628095</v>
+      </c>
+      <c r="H29" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="K29" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="L29" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="M29" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="N29" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="O29" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="P29" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q29" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R29" s="63">
+        <v>201480</v>
+      </c>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
@@ -9809,15 +11036,8 @@
       <c r="A948" s="11"/>
       <c r="G948" s="11"/>
     </row>
-    <row r="949" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A949" s="11"/>
-      <c r="G949" s="11"/>
-    </row>
-    <row r="950" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A950" s="11"/>
-      <c r="G950" s="11"/>
-    </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9825,10 +11045,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N952"/>
+  <dimension ref="A1:N950"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10368,8 +11588,8 @@
       <c r="G14" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>128</v>
+      <c r="H14" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="I14" s="2">
         <v>1</v>
@@ -10406,8 +11626,8 @@
       <c r="G15" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>128</v>
+      <c r="H15" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="I15" s="2">
         <v>1</v>
@@ -10444,8 +11664,8 @@
       <c r="G16" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>128</v>
+      <c r="H16" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="I16" s="2">
         <v>1</v>
@@ -10482,8 +11702,8 @@
       <c r="G17" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>128</v>
+      <c r="H17" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="I17" s="2">
         <v>1</v>
@@ -10520,8 +11740,8 @@
       <c r="G18" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>128</v>
+      <c r="H18" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="I18" s="2">
         <v>1</v>
@@ -10558,8 +11778,8 @@
       <c r="G19" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>128</v>
+      <c r="H19" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="I19" s="2">
         <v>1</v>
@@ -10580,35 +11800,437 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="57">
+        <v>6628084</v>
+      </c>
+      <c r="B20" s="57"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" s="58" t="str">
+        <f t="shared" ref="G20:G29" si="0">CONCATENATE(F20,"Sp")</f>
+        <v>Lin6628084Sp</v>
+      </c>
+      <c r="H20" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="I20" s="58">
+        <v>1</v>
+      </c>
+      <c r="J20" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K20" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N20" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="57">
+        <v>6628085</v>
+      </c>
+      <c r="B21" s="57"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>Lin6628085Sp</v>
+      </c>
+      <c r="H21" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="58">
+        <v>1</v>
+      </c>
+      <c r="J21" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K21" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L21" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="M21" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N21" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="57">
+        <v>6628087</v>
+      </c>
+      <c r="B22" s="57"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>Lin6628087Sp</v>
+      </c>
+      <c r="H22" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" s="58">
+        <v>1</v>
+      </c>
+      <c r="J22" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K22" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="M22" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N22" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="57">
+        <v>6628088</v>
+      </c>
+      <c r="B23" s="57"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="G23" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>Lin6628088Sp</v>
+      </c>
+      <c r="H23" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" s="58">
+        <v>1</v>
+      </c>
+      <c r="J23" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K23" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L23" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N23" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="57">
+        <v>6628090</v>
+      </c>
+      <c r="B24" s="57"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="G24" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>Lin6628090Sp</v>
+      </c>
+      <c r="H24" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24" s="58">
+        <v>1</v>
+      </c>
+      <c r="J24" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K24" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L24" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="M24" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N24" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="57">
+        <v>6628091</v>
+      </c>
+      <c r="B25" s="57"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>Lin6628091Sp</v>
+      </c>
+      <c r="H25" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="I25" s="58">
+        <v>1</v>
+      </c>
+      <c r="J25" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K25" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L25" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="M25" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N25" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="57">
+        <v>6628071</v>
+      </c>
+      <c r="B26" s="57"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>Lin6628071Sp</v>
+      </c>
+      <c r="H26" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="I26" s="58">
+        <v>1</v>
+      </c>
+      <c r="J26" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K26" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L26" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="M26" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N26" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="57">
+        <v>6628092</v>
+      </c>
+      <c r="B27" s="57"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="G27" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>Lin6628092Sp</v>
+      </c>
+      <c r="H27" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="I27" s="58">
+        <v>1</v>
+      </c>
+      <c r="J27" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K27" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L27" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="M27" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N27" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="57">
+        <v>6628094</v>
+      </c>
+      <c r="B28" s="57"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>Lin6628094Sp</v>
+      </c>
+      <c r="H28" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="I28" s="58">
+        <v>1</v>
+      </c>
+      <c r="J28" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K28" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L28" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="M28" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N28" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="57">
+        <v>6628095</v>
+      </c>
+      <c r="B29" s="57"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>Lin6628095Sp</v>
+      </c>
+      <c r="H29" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="I29" s="58">
+        <v>1</v>
+      </c>
+      <c r="J29" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="K29" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="L29" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="M29" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="N29" s="61">
+        <v>201480</v>
+      </c>
+    </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11511,8 +13133,6 @@
     <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11521,10 +13141,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB956"/>
+  <dimension ref="A1:AB954"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12234,7 +13854,7 @@
         <v>1254</v>
       </c>
       <c r="P14" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="Q14" s="26" t="s">
         <v>67</v>
@@ -12282,7 +13902,7 @@
         <v>1254</v>
       </c>
       <c r="P15" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="Q15" s="26" t="s">
         <v>67</v>
@@ -12333,7 +13953,7 @@
         <v>1254</v>
       </c>
       <c r="P16" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="Q16" s="26" t="s">
         <v>67</v>
@@ -12381,7 +14001,7 @@
         <v>1254</v>
       </c>
       <c r="P17" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="Q17" s="26" t="s">
         <v>67</v>
@@ -12429,7 +14049,7 @@
         <v>1254</v>
       </c>
       <c r="P18" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="Q18" s="26" t="s">
         <v>67</v>
@@ -12480,7 +14100,7 @@
         <v>1254</v>
       </c>
       <c r="P19" s="26" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="Q19" s="26" t="s">
         <v>67</v>
@@ -12490,21 +14110,509 @@
       </c>
       <c r="S19" s="35"/>
     </row>
-    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="57">
+        <v>6628084</v>
+      </c>
+      <c r="B20" s="57"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" s="59"/>
+      <c r="M20" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N20" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O20" s="61">
+        <v>1254</v>
+      </c>
+      <c r="P20" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q20" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R20" s="61">
+        <v>201480</v>
+      </c>
+    </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="10"/>
+      <c r="A21" s="57">
+        <v>6628085</v>
+      </c>
+      <c r="B21" s="57"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="61" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="F21" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="L21" s="59"/>
+      <c r="M21" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N21" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O21" s="61">
+        <v>1254</v>
+      </c>
+      <c r="P21" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q21" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R21" s="61">
+        <v>201480</v>
+      </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="A22" s="57">
+        <v>6628087</v>
+      </c>
+      <c r="B22" s="57"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K22" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="L22" s="59"/>
+      <c r="M22" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N22" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O22" s="61">
+        <v>1254</v>
+      </c>
+      <c r="P22" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q22" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R22" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="57">
+        <v>6628088</v>
+      </c>
+      <c r="B23" s="57"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K23" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="L23" s="59"/>
+      <c r="M23" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N23" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O23" s="61">
+        <v>1254</v>
+      </c>
+      <c r="P23" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q23" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R23" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="57">
+        <v>6628090</v>
+      </c>
+      <c r="B24" s="57"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="I24" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="K24" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="L24" s="59"/>
+      <c r="M24" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N24" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O24" s="61">
+        <v>1254</v>
+      </c>
+      <c r="P24" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q24" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R24" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="57">
+        <v>6628091</v>
+      </c>
+      <c r="B25" s="57"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="I25" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="L25" s="59"/>
+      <c r="M25" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N25" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O25" s="61">
+        <v>1254</v>
+      </c>
+      <c r="P25" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q25" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R25" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="57">
+        <v>6628071</v>
+      </c>
+      <c r="B26" s="57"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="58" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="I26" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="K26" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="L26" s="59"/>
+      <c r="M26" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N26" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O26" s="61">
+        <v>1254</v>
+      </c>
+      <c r="P26" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q26" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R26" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="57">
+        <v>6628092</v>
+      </c>
+      <c r="B27" s="57"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="I27" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K27" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="L27" s="59"/>
+      <c r="M27" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N27" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O27" s="61">
+        <v>1254</v>
+      </c>
+      <c r="P27" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q27" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R27" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="57">
+        <v>6628094</v>
+      </c>
+      <c r="B28" s="57"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="I28" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="K28" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="L28" s="59"/>
+      <c r="M28" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N28" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O28" s="61">
+        <v>1254</v>
+      </c>
+      <c r="P28" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q28" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R28" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="57">
+        <v>6628095</v>
+      </c>
+      <c r="B29" s="57"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="F29" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="H29" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="I29" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="K29" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="L29" s="59"/>
+      <c r="M29" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="N29" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="O29" s="61">
+        <v>1254</v>
+      </c>
+      <c r="P29" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q29" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R29" s="61">
+        <v>201480</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="10"/>
+    </row>
     <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13429,8 +15537,6 @@
     <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Work on Lease Creation [Active /Inactive Issue
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3391" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3429" uniqueCount="278">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -849,13 +849,13 @@
     <t>Reg2ndRevExSp4160</t>
   </si>
   <si>
-    <t>Reg2ndRevExSp4161</t>
-  </si>
-  <si>
-    <t>Reg2ndRevEx4161</t>
-  </si>
-  <si>
-    <t>Fiscal Year</t>
+    <t>Reg2ndRevEx4162</t>
+  </si>
+  <si>
+    <t>Reg2ndRevExSp4162</t>
+  </si>
+  <si>
+    <t>Lease Year</t>
   </si>
 </sst>
 </file>
@@ -1813,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="K76" sqref="K76"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5050,7 +5050,7 @@
         <v>270</v>
       </c>
       <c r="O71" s="59" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="P71" s="54" t="s">
         <v>60</v>
@@ -5061,15 +5061,15 @@
     </row>
     <row r="72" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
       <c r="A72" s="114">
-        <v>6624161</v>
+        <v>6624162</v>
       </c>
       <c r="B72" s="53"/>
       <c r="C72" s="53"/>
       <c r="D72" s="108" t="s">
+        <v>275</v>
+      </c>
+      <c r="E72" s="107" t="s">
         <v>276</v>
-      </c>
-      <c r="E72" s="107" t="s">
-        <v>275</v>
       </c>
       <c r="F72" s="19" t="s">
         <v>197</v>
@@ -5078,7 +5078,7 @@
         <v>196</v>
       </c>
       <c r="H72" s="53" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="I72" s="54" t="s">
         <v>34</v>
@@ -6039,8 +6039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y986"/>
   <sheetViews>
-    <sheetView topLeftCell="J58" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView topLeftCell="I58" workbookViewId="0">
+      <selection activeCell="T73" sqref="T73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -10271,7 +10271,7 @@
         <v>1</v>
       </c>
       <c r="T73" s="59" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="U73" s="57" t="s">
         <v>60</v>
@@ -10280,8 +10280,69 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A74" s="4"/>
+    <row r="74" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A74" s="114">
+        <v>6624162</v>
+      </c>
+      <c r="B74" s="57"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="E74" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="F74" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="G74" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="H74" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="69">
+        <v>12230</v>
+      </c>
+      <c r="J74" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="K74" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="L74" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="M74" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="N74" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="O74" s="69">
+        <v>100000000</v>
+      </c>
+      <c r="P74" s="57" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q74" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="R74" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="S74" s="70" t="b">
+        <v>1</v>
+      </c>
+      <c r="T74" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U74" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="V74" s="69">
+        <v>201480</v>
+      </c>
     </row>
     <row r="75" spans="1:22" ht="15.75" customHeight="1">
       <c r="A75" s="4"/>
@@ -13034,8 +13095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R981"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -16478,7 +16539,7 @@
         <v>65</v>
       </c>
       <c r="N74" s="75" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="O74" s="57" t="s">
         <v>61</v>
@@ -16493,9 +16554,57 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A75" s="12"/>
-      <c r="G75" s="12"/>
+    <row r="75" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A75" s="114">
+        <v>6624162</v>
+      </c>
+      <c r="B75" s="57"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="E75" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="F75" s="108" t="s">
+        <v>275</v>
+      </c>
+      <c r="G75" s="108" t="s">
+        <v>275</v>
+      </c>
+      <c r="H75" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="I75" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="J75" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="K75" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="L75" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="M75" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="N75" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="O75" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="P75" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q75" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="R75" s="53">
+        <v>201480</v>
+      </c>
     </row>
     <row r="76" spans="1:18" ht="15.75" customHeight="1">
       <c r="A76" s="12"/>
@@ -20136,8 +20245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD983"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -22795,7 +22904,7 @@
         <v>274</v>
       </c>
       <c r="H72" s="109" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="I72" s="110">
         <v>1</v>
@@ -22816,7 +22925,46 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A73" s="114">
+        <v>6624162</v>
+      </c>
+      <c r="B73" s="107"/>
+      <c r="C73" s="107"/>
+      <c r="D73" s="108" t="s">
+        <v>261</v>
+      </c>
+      <c r="E73" s="108" t="s">
+        <v>261</v>
+      </c>
+      <c r="F73" s="108" t="s">
+        <v>275</v>
+      </c>
+      <c r="G73" s="107" t="s">
+        <v>276</v>
+      </c>
+      <c r="H73" s="109" t="s">
+        <v>54</v>
+      </c>
+      <c r="I73" s="110">
+        <v>1</v>
+      </c>
+      <c r="J73" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="K73" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="L73" s="111" t="s">
+        <v>99</v>
+      </c>
+      <c r="M73" s="107" t="s">
+        <v>60</v>
+      </c>
+      <c r="N73" s="53">
+        <v>201480</v>
+      </c>
+    </row>
     <row r="74" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="75" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="76" spans="1:14" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
partial complete test cases of 2nd revision
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4050" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="4500" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3429" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3480" uniqueCount="280">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -856,6 +856,12 @@
   </si>
   <si>
     <t>Lease Year</t>
+  </si>
+  <si>
+    <t>Reg2ndRevEx4161</t>
+  </si>
+  <si>
+    <t>Reg2ndRevExSp4161</t>
   </si>
 </sst>
 </file>
@@ -1814,7 +1820,7 @@
   <dimension ref="A1:AA988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+      <selection activeCell="O72" sqref="O72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5099,7 +5105,7 @@
         <v>270</v>
       </c>
       <c r="O72" s="59" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="P72" s="54" t="s">
         <v>60</v>
@@ -5108,7 +5114,55 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="73" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A73" s="114">
+        <v>6624161</v>
+      </c>
+      <c r="B73" s="53"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="108" t="s">
+        <v>278</v>
+      </c>
+      <c r="E73" s="107" t="s">
+        <v>279</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="G73" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="H73" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="I73" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="J73" s="54" t="s">
+        <v>266</v>
+      </c>
+      <c r="K73" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="L73" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="M73" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="N73" s="55" t="s">
+        <v>270</v>
+      </c>
+      <c r="O73" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="P73" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q73" s="53">
+        <v>201480</v>
+      </c>
+    </row>
     <row r="74" spans="1:17" ht="15.75" customHeight="1"/>
     <row r="75" spans="1:17" ht="15.75" customHeight="1"/>
     <row r="76" spans="1:17" ht="15.75" customHeight="1"/>
@@ -6039,8 +6093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y986"/>
   <sheetViews>
-    <sheetView topLeftCell="I58" workbookViewId="0">
-      <selection activeCell="T73" sqref="T73"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="T74" sqref="T74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -10335,7 +10389,7 @@
         <v>1</v>
       </c>
       <c r="T74" s="59" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="U74" s="57" t="s">
         <v>60</v>
@@ -10344,8 +10398,69 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A75" s="4"/>
+    <row r="75" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A75" s="114">
+        <v>6624161</v>
+      </c>
+      <c r="B75" s="57"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="E75" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="F75" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="G75" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="H75" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="I75" s="69">
+        <v>12230</v>
+      </c>
+      <c r="J75" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="K75" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="L75" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="M75" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="N75" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="O75" s="69">
+        <v>100000000</v>
+      </c>
+      <c r="P75" s="57" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q75" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="R75" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="S75" s="70" t="b">
+        <v>1</v>
+      </c>
+      <c r="T75" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U75" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="V75" s="69">
+        <v>201480</v>
+      </c>
     </row>
     <row r="76" spans="1:22" ht="15.75" customHeight="1">
       <c r="A76" s="4"/>
@@ -13095,8 +13210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R981"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView topLeftCell="E58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N75" sqref="N75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -16591,7 +16706,7 @@
         <v>65</v>
       </c>
       <c r="N75" s="75" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="O75" s="57" t="s">
         <v>61</v>
@@ -16606,9 +16721,57 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A76" s="12"/>
-      <c r="G76" s="12"/>
+    <row r="76" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A76" s="114">
+        <v>6624161</v>
+      </c>
+      <c r="B76" s="57"/>
+      <c r="C76" s="57"/>
+      <c r="D76" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="E76" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="F76" s="108" t="s">
+        <v>278</v>
+      </c>
+      <c r="G76" s="108" t="s">
+        <v>278</v>
+      </c>
+      <c r="H76" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="I76" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="J76" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="K76" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="L76" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="M76" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="N76" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="O76" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="P76" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q76" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="R76" s="53">
+        <v>201480</v>
+      </c>
     </row>
     <row r="77" spans="1:18" ht="15.75" customHeight="1">
       <c r="A77" s="12"/>
@@ -20246,7 +20409,7 @@
   <dimension ref="A1:AD983"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -22944,7 +23107,7 @@
         <v>276</v>
       </c>
       <c r="H73" s="109" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
       <c r="I73" s="110">
         <v>1</v>
@@ -22965,7 +23128,46 @@
         <v>201480</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="74" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A74" s="114">
+        <v>6624161</v>
+      </c>
+      <c r="B74" s="107"/>
+      <c r="C74" s="107"/>
+      <c r="D74" s="108" t="s">
+        <v>261</v>
+      </c>
+      <c r="E74" s="108" t="s">
+        <v>261</v>
+      </c>
+      <c r="F74" s="108" t="s">
+        <v>278</v>
+      </c>
+      <c r="G74" s="107" t="s">
+        <v>279</v>
+      </c>
+      <c r="H74" s="109" t="s">
+        <v>54</v>
+      </c>
+      <c r="I74" s="110">
+        <v>1</v>
+      </c>
+      <c r="J74" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="K74" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="L74" s="111" t="s">
+        <v>99</v>
+      </c>
+      <c r="M74" s="107" t="s">
+        <v>60</v>
+      </c>
+      <c r="N74" s="53">
+        <v>201480</v>
+      </c>
+    </row>
     <row r="75" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="76" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="77" spans="1:14" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
New Method added at UIDrop Down
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/DataCreate.xlsx
+++ b/src/main/resources/dataCreate/DataCreate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asif/Documents/AMT-TestFrameWork/src/main/resources/dataCreate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7072EDEC-1D16-B444-9E93-D9342F8B4510}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16AC3DE-3C7E-B04B-B9A1-ADE1E43DA3DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="93">
   <si>
     <t>Reference_TcID</t>
   </si>
@@ -260,16 +260,10 @@
     <t>fiscalYear</t>
   </si>
   <si>
-    <t>FRAT  : Lessee Test Cases</t>
-  </si>
-  <si>
     <t>1234</t>
   </si>
   <si>
     <t>10000</t>
-  </si>
-  <si>
-    <t>Schedule</t>
   </si>
   <si>
     <t>ScheduleEx</t>
@@ -278,73 +272,43 @@
     <t>ScheduleEx6545928</t>
   </si>
   <si>
-    <t>Schedule6546535</t>
-  </si>
-  <si>
-    <t>Schedule6596614</t>
-  </si>
-  <si>
-    <t>Schedule6596618</t>
-  </si>
-  <si>
     <t>ScheduleEx6596772</t>
-  </si>
-  <si>
-    <t>Schedule6596919</t>
-  </si>
-  <si>
-    <t>Schedule6598612</t>
-  </si>
-  <si>
-    <t>Schedule6598662</t>
   </si>
   <si>
     <t>ScheduleEx6597034</t>
   </si>
   <si>
-    <t>Schedule6598609</t>
+    <t>SMOKE : Schedule Test Cases</t>
   </si>
   <si>
-    <t>Schedule6598809</t>
+    <t>ScheduleIn</t>
   </si>
   <si>
-    <t>Schedule6598923</t>
+    <t>ScheduleIn6546535</t>
   </si>
   <si>
-    <t>ScheduleEx6545928Sp</t>
+    <t>ScheduleIn6596614</t>
   </si>
   <si>
-    <t>Schedule6546535Sp</t>
+    <t>ScheduleIn6596618</t>
   </si>
   <si>
-    <t>Schedule6596614Sp</t>
+    <t>ScheduleIn6596919</t>
   </si>
   <si>
-    <t>Schedule6596618Sp</t>
+    <t>ScheduleIn6598612</t>
   </si>
   <si>
-    <t>ScheduleEx6596772Sp</t>
+    <t>ScheduleIn6598662</t>
   </si>
   <si>
-    <t>Schedule6596919Sp</t>
+    <t>ScheduleIn6598609</t>
   </si>
   <si>
-    <t>Schedule6598612Sp</t>
+    <t>ScheduleIn6598809</t>
   </si>
   <si>
-    <t>Schedule6598662Sp</t>
-  </si>
-  <si>
-    <t>ScheduleEx6597034Sp</t>
-  </si>
-  <si>
-    <t>Schedule6598609Sp</t>
-  </si>
-  <si>
-    <t>Schedule6598809Sp</t>
-  </si>
-  <si>
-    <t>Schedule6598923Sp</t>
+    <t>ScheduleIn6598923</t>
   </si>
 </sst>
 </file>
@@ -530,7 +494,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -571,7 +535,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -980,14 +943,14 @@
   <dimension ref="A1:Y902"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
@@ -1080,32 +1043,32 @@
       <c r="Y1" s="2"/>
     </row>
     <row r="2" spans="1:25" ht="16" thickBot="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="27" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
@@ -1115,60 +1078,60 @@
         <v>6545928</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="24">
         <v>12230</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="31" t="s">
+      <c r="N3" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="25">
+      <c r="O3" s="24">
         <v>100000000</v>
       </c>
-      <c r="P3" s="25" t="s">
+      <c r="P3" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="Q3" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="22" t="s">
+      <c r="R3" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S3" s="25" t="b">
+      <c r="S3" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T3" s="22" t="s">
+      <c r="T3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U3" s="22" t="s">
+      <c r="U3" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V3" s="32">
+      <c r="V3" s="31">
         <v>201480</v>
       </c>
       <c r="W3" s="2"/>
@@ -1180,60 +1143,60 @@
         <v>6546535</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="24">
         <v>12230</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="31" t="s">
+      <c r="N4" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="25">
+      <c r="O4" s="24">
         <v>100000000</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q4" s="31" t="s">
+      <c r="Q4" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R4" s="22" t="s">
+      <c r="R4" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S4" s="25" t="b">
+      <c r="S4" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T4" s="22" t="s">
+      <c r="T4" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U4" s="22" t="s">
+      <c r="U4" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V4" s="32">
+      <c r="V4" s="31">
         <v>201480</v>
       </c>
       <c r="W4" s="2"/>
@@ -1245,60 +1208,60 @@
         <v>6596614</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="24">
         <v>12230</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O5" s="25">
+      <c r="O5" s="24">
         <v>100000000</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="P5" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q5" s="31" t="s">
+      <c r="Q5" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="R5" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S5" s="25" t="b">
+      <c r="S5" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T5" s="22" t="s">
+      <c r="T5" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U5" s="22" t="s">
+      <c r="U5" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V5" s="32">
+      <c r="V5" s="31">
         <v>201480</v>
       </c>
       <c r="W5" s="2"/>
@@ -1310,60 +1273,60 @@
         <v>6596618</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="24">
         <v>12230</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="25" t="s">
+      <c r="K6" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="25" t="s">
+      <c r="M6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O6" s="25">
+      <c r="O6" s="24">
         <v>100000000</v>
       </c>
-      <c r="P6" s="25" t="s">
+      <c r="P6" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" s="31" t="s">
+      <c r="Q6" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="22" t="s">
+      <c r="R6" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S6" s="25" t="b">
+      <c r="S6" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T6" s="22" t="s">
+      <c r="T6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U6" s="22" t="s">
+      <c r="U6" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V6" s="32">
+      <c r="V6" s="31">
         <v>201480</v>
       </c>
       <c r="W6" s="2"/>
@@ -1371,64 +1334,64 @@
       <c r="Y6" s="2"/>
     </row>
     <row r="7" spans="1:25">
-      <c r="A7" s="29">
+      <c r="A7" s="28">
         <v>6596772</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="24">
         <v>12230</v>
       </c>
-      <c r="J7" s="25" t="s">
+      <c r="J7" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="K7" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="L7" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="M7" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="31" t="s">
+      <c r="N7" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7" s="24">
         <v>100000000</v>
       </c>
-      <c r="P7" s="25" t="s">
+      <c r="P7" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q7" s="31" t="s">
+      <c r="Q7" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R7" s="22" t="s">
+      <c r="R7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S7" s="25" t="b">
+      <c r="S7" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T7" s="22" t="s">
+      <c r="T7" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U7" s="22" t="s">
+      <c r="U7" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V7" s="32">
+      <c r="V7" s="31">
         <v>201481</v>
       </c>
       <c r="W7" s="2"/>
@@ -1436,64 +1399,64 @@
       <c r="Y7" s="2"/>
     </row>
     <row r="8" spans="1:25">
-      <c r="A8" s="29">
+      <c r="A8" s="28">
         <v>6596919</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="24">
         <v>12230</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="L8" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="25" t="s">
+      <c r="M8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="31" t="s">
+      <c r="N8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="25">
+      <c r="O8" s="24">
         <v>100000000</v>
       </c>
-      <c r="P8" s="25" t="s">
+      <c r="P8" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q8" s="31" t="s">
+      <c r="Q8" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R8" s="22" t="s">
+      <c r="R8" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S8" s="25" t="b">
+      <c r="S8" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T8" s="22" t="s">
+      <c r="T8" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U8" s="22" t="s">
+      <c r="U8" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V8" s="32">
+      <c r="V8" s="31">
         <v>201481</v>
       </c>
       <c r="W8" s="2"/>
@@ -1501,64 +1464,64 @@
       <c r="Y8" s="2"/>
     </row>
     <row r="9" spans="1:25">
-      <c r="A9" s="29">
+      <c r="A9" s="28">
         <v>6598612</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="24">
         <v>12230</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="25" t="s">
+      <c r="K9" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L9" s="25" t="s">
+      <c r="L9" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="25" t="s">
+      <c r="M9" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="31" t="s">
+      <c r="N9" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="25">
+      <c r="O9" s="24">
         <v>100000000</v>
       </c>
-      <c r="P9" s="25" t="s">
+      <c r="P9" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q9" s="31" t="s">
+      <c r="Q9" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R9" s="22" t="s">
+      <c r="R9" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S9" s="25" t="b">
+      <c r="S9" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T9" s="22" t="s">
+      <c r="T9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U9" s="22" t="s">
+      <c r="U9" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V9" s="32">
+      <c r="V9" s="31">
         <v>201481</v>
       </c>
       <c r="W9" s="2"/>
@@ -1566,64 +1529,64 @@
       <c r="Y9" s="2"/>
     </row>
     <row r="10" spans="1:25">
-      <c r="A10" s="29">
+      <c r="A10" s="28">
         <v>6598662</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="24">
         <v>12230</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="25" t="s">
+      <c r="K10" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="25" t="s">
+      <c r="M10" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N10" s="31" t="s">
+      <c r="N10" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O10" s="25">
+      <c r="O10" s="24">
         <v>100000000</v>
       </c>
-      <c r="P10" s="25" t="s">
+      <c r="P10" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q10" s="31" t="s">
+      <c r="Q10" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R10" s="22" t="s">
+      <c r="R10" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S10" s="25" t="b">
+      <c r="S10" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T10" s="22" t="s">
+      <c r="T10" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U10" s="22" t="s">
+      <c r="U10" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V10" s="32">
+      <c r="V10" s="31">
         <v>201481</v>
       </c>
       <c r="W10" s="2"/>
@@ -1635,60 +1598,60 @@
         <v>6597034</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="24">
         <v>12230</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="25" t="s">
+      <c r="K11" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="L11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="25" t="s">
+      <c r="M11" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="31" t="s">
+      <c r="N11" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="25">
+      <c r="O11" s="24">
         <v>100000000</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="P11" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q11" s="31" t="s">
+      <c r="Q11" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R11" s="22" t="s">
+      <c r="R11" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S11" s="25" t="b">
+      <c r="S11" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T11" s="22" t="s">
+      <c r="T11" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U11" s="22" t="s">
+      <c r="U11" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V11" s="32">
+      <c r="V11" s="31">
         <v>201482</v>
       </c>
       <c r="W11" s="2"/>
@@ -1700,60 +1663,60 @@
         <v>6598609</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="24">
         <v>12230</v>
       </c>
-      <c r="J12" s="25" t="s">
+      <c r="J12" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="25" t="s">
+      <c r="K12" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L12" s="25" t="s">
+      <c r="L12" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="25" t="s">
+      <c r="M12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N12" s="31" t="s">
+      <c r="N12" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O12" s="25">
+      <c r="O12" s="24">
         <v>100000000</v>
       </c>
-      <c r="P12" s="25" t="s">
+      <c r="P12" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q12" s="31" t="s">
+      <c r="Q12" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R12" s="22" t="s">
+      <c r="R12" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S12" s="25" t="b">
+      <c r="S12" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T12" s="22" t="s">
+      <c r="T12" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U12" s="22" t="s">
+      <c r="U12" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V12" s="32">
+      <c r="V12" s="31">
         <v>201482</v>
       </c>
       <c r="W12" s="2"/>
@@ -1765,60 +1728,60 @@
         <v>6598809</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="24">
         <v>12230</v>
       </c>
-      <c r="J13" s="25" t="s">
+      <c r="J13" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="25" t="s">
+      <c r="K13" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="25" t="s">
+      <c r="M13" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N13" s="31" t="s">
+      <c r="N13" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="24">
         <v>100000000</v>
       </c>
-      <c r="P13" s="25" t="s">
+      <c r="P13" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q13" s="31" t="s">
+      <c r="Q13" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R13" s="22" t="s">
+      <c r="R13" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S13" s="25" t="b">
+      <c r="S13" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T13" s="22" t="s">
+      <c r="T13" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U13" s="22" t="s">
+      <c r="U13" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V13" s="32">
+      <c r="V13" s="31">
         <v>201482</v>
       </c>
       <c r="W13" s="2"/>
@@ -1830,60 +1793,60 @@
         <v>6598923</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="24">
         <v>12230</v>
       </c>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="25" t="s">
+      <c r="K14" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="L14" s="25" t="s">
+      <c r="L14" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="25" t="s">
+      <c r="M14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="N14" s="31" t="s">
+      <c r="N14" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="O14" s="25">
+      <c r="O14" s="24">
         <v>100000000</v>
       </c>
-      <c r="P14" s="25" t="s">
+      <c r="P14" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Q14" s="31" t="s">
+      <c r="Q14" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="R14" s="22" t="s">
+      <c r="R14" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S14" s="25" t="b">
+      <c r="S14" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="T14" s="22" t="s">
+      <c r="T14" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="U14" s="22" t="s">
+      <c r="U14" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="V14" s="32">
+      <c r="V14" s="31">
         <v>201482</v>
       </c>
       <c r="W14" s="2"/>
@@ -4569,15 +4532,15 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:R888"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="17" style="6" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="6" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
     <col min="6" max="6" width="19.5" style="6" customWidth="1"/>
@@ -4653,56 +4616,56 @@
       </c>
     </row>
     <row r="2" spans="1:18" s="13" customFormat="1">
-      <c r="A2" s="29">
+      <c r="A2" s="28">
         <v>6545928</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
       <c r="D2" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="22" t="str">
+        <v>78</v>
+      </c>
+      <c r="F2" s="21" t="str">
         <f>CONCATENATE(E2,A2)</f>
         <v>ScheduleEx6545928</v>
       </c>
-      <c r="G2" s="22" t="str">
+      <c r="G2" s="21" t="str">
         <f>CONCATENATE(F2,B2)</f>
         <v>ScheduleEx6545928</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="N2" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="O2" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="P2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="R2" s="21">
+      <c r="R2" s="20">
         <v>201480</v>
       </c>
     </row>
@@ -4710,53 +4673,53 @@
       <c r="A3" s="15">
         <v>6546535</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="22" t="str">
+        <v>83</v>
+      </c>
+      <c r="F3" s="21" t="str">
         <f t="shared" ref="F3:G13" si="0">CONCATENATE(E3,A3)</f>
-        <v>Schedule6546535</v>
-      </c>
-      <c r="G3" s="22" t="str">
+        <v>ScheduleIn6546535</v>
+      </c>
+      <c r="G3" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6546535</v>
-      </c>
-      <c r="H3" s="22" t="s">
+        <v>ScheduleIn6546535</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N3" s="33" t="s">
+      <c r="N3" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="R3" s="21">
+      <c r="R3" s="20">
         <v>201480</v>
       </c>
     </row>
@@ -4764,53 +4727,53 @@
       <c r="A4" s="15">
         <v>6596614</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="22" t="str">
+        <v>83</v>
+      </c>
+      <c r="F4" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6596614</v>
-      </c>
-      <c r="G4" s="22" t="str">
+        <v>ScheduleIn6596614</v>
+      </c>
+      <c r="G4" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6596614</v>
-      </c>
-      <c r="H4" s="22" t="s">
+        <v>ScheduleIn6596614</v>
+      </c>
+      <c r="H4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N4" s="33" t="s">
+      <c r="N4" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="21">
+      <c r="R4" s="20">
         <v>201480</v>
       </c>
     </row>
@@ -4818,313 +4781,313 @@
       <c r="A5" s="15">
         <v>6596618</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="22" t="str">
+        <v>83</v>
+      </c>
+      <c r="F5" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6596618</v>
-      </c>
-      <c r="G5" s="22" t="str">
+        <v>ScheduleIn6596618</v>
+      </c>
+      <c r="G5" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6596618</v>
-      </c>
-      <c r="H5" s="22" t="s">
+        <v>ScheduleIn6596618</v>
+      </c>
+      <c r="H5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="L5" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N5" s="33" t="s">
+      <c r="N5" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="24" t="s">
+      <c r="O5" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="P5" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="R5" s="21">
+      <c r="R5" s="20">
         <v>201480</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A6" s="29">
+      <c r="A6" s="28">
         <v>6596772</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="22" t="str">
+        <v>78</v>
+      </c>
+      <c r="F6" s="21" t="str">
         <f t="shared" si="0"/>
         <v>ScheduleEx6596772</v>
       </c>
-      <c r="G6" s="22" t="str">
+      <c r="G6" s="21" t="str">
         <f t="shared" si="0"/>
         <v>ScheduleEx6596772</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="K6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="N6" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="24" t="s">
+      <c r="O6" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="P6" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="Q6" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="R6" s="21">
+      <c r="R6" s="20">
         <v>201481</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A7" s="28">
+      <c r="A7" s="27">
         <v>6596919</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="22" t="str">
+        <v>83</v>
+      </c>
+      <c r="F7" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6596919</v>
-      </c>
-      <c r="G7" s="22" t="str">
+        <v>ScheduleIn6596919</v>
+      </c>
+      <c r="G7" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6596919</v>
-      </c>
-      <c r="H7" s="22" t="s">
+        <v>ScheduleIn6596919</v>
+      </c>
+      <c r="H7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="24" t="s">
+      <c r="L7" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="33" t="s">
+      <c r="N7" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="O7" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="P7" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q7" s="45" t="s">
+      <c r="Q7" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="R7" s="21">
+      <c r="R7" s="20">
         <v>201481</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A8" s="28">
+      <c r="A8" s="27">
         <v>6598612</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="22" t="str">
+        <v>83</v>
+      </c>
+      <c r="F8" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6598612</v>
-      </c>
-      <c r="G8" s="22" t="str">
+        <v>ScheduleIn6598612</v>
+      </c>
+      <c r="G8" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6598612</v>
-      </c>
-      <c r="H8" s="22" t="s">
+        <v>ScheduleIn6598612</v>
+      </c>
+      <c r="H8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="24" t="s">
+      <c r="K8" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="24" t="s">
+      <c r="L8" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="M8" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N8" s="33" t="s">
+      <c r="N8" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O8" s="24" t="s">
+      <c r="O8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="P8" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q8" s="45" t="s">
+      <c r="Q8" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="R8" s="21">
+      <c r="R8" s="20">
         <v>201481</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A9" s="28">
+      <c r="A9" s="27">
         <v>6598662</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="22" t="str">
+        <v>83</v>
+      </c>
+      <c r="F9" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6598662</v>
-      </c>
-      <c r="G9" s="22" t="str">
+        <v>ScheduleIn6598662</v>
+      </c>
+      <c r="G9" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6598662</v>
-      </c>
-      <c r="H9" s="22" t="s">
+        <v>ScheduleIn6598662</v>
+      </c>
+      <c r="H9" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K9" s="24" t="s">
+      <c r="K9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="M9" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="33" t="s">
+      <c r="N9" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="24" t="s">
+      <c r="O9" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P9" s="24" t="s">
+      <c r="P9" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q9" s="45" t="s">
+      <c r="Q9" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="R9" s="21">
+      <c r="R9" s="20">
         <v>201481</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A10" s="29">
+      <c r="A10" s="28">
         <v>6597034</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="22" t="str">
+        <v>78</v>
+      </c>
+      <c r="F10" s="21" t="str">
         <f t="shared" si="0"/>
         <v>ScheduleEx6597034</v>
       </c>
-      <c r="G10" s="22" t="str">
+      <c r="G10" s="21" t="str">
         <f t="shared" si="0"/>
         <v>ScheduleEx6597034</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="K10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="24" t="s">
+      <c r="L10" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="M10" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N10" s="33" t="s">
+      <c r="N10" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O10" s="24" t="s">
+      <c r="O10" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P10" s="24" t="s">
+      <c r="P10" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q10" s="45" t="s">
+      <c r="Q10" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="R10" s="21">
+      <c r="R10" s="20">
         <v>201482</v>
       </c>
     </row>
@@ -5133,50 +5096,50 @@
         <v>6598609</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="22" t="str">
+        <v>83</v>
+      </c>
+      <c r="F11" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6598609</v>
-      </c>
-      <c r="G11" s="22" t="str">
+        <v>ScheduleIn6598609</v>
+      </c>
+      <c r="G11" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6598609</v>
-      </c>
-      <c r="H11" s="22" t="s">
+        <v>ScheduleIn6598609</v>
+      </c>
+      <c r="H11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="24" t="s">
+      <c r="K11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="24" t="s">
+      <c r="L11" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="M11" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N11" s="33" t="s">
+      <c r="N11" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O11" s="24" t="s">
+      <c r="O11" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="P11" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q11" s="45" t="s">
+      <c r="Q11" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="R11" s="21">
+      <c r="R11" s="20">
         <v>201482</v>
       </c>
     </row>
@@ -5185,50 +5148,50 @@
         <v>6598809</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="22" t="str">
+        <v>83</v>
+      </c>
+      <c r="F12" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6598809</v>
-      </c>
-      <c r="G12" s="22" t="str">
+        <v>ScheduleIn6598809</v>
+      </c>
+      <c r="G12" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6598809</v>
-      </c>
-      <c r="H12" s="22" t="s">
+        <v>ScheduleIn6598809</v>
+      </c>
+      <c r="H12" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K12" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="24" t="s">
+      <c r="L12" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="M12" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N12" s="33" t="s">
+      <c r="N12" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O12" s="24" t="s">
+      <c r="O12" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P12" s="24" t="s">
+      <c r="P12" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q12" s="45" t="s">
+      <c r="Q12" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="R12" s="21">
+      <c r="R12" s="20">
         <v>201482</v>
       </c>
     </row>
@@ -5237,50 +5200,50 @@
         <v>6598923</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="22" t="str">
+        <v>83</v>
+      </c>
+      <c r="F13" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6598923</v>
-      </c>
-      <c r="G13" s="22" t="str">
+        <v>ScheduleIn6598923</v>
+      </c>
+      <c r="G13" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>Schedule6598923</v>
-      </c>
-      <c r="H13" s="22" t="s">
+        <v>ScheduleIn6598923</v>
+      </c>
+      <c r="H13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="K13" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="24" t="s">
+      <c r="L13" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="M13" s="17" t="s">
+      <c r="M13" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="33" t="s">
+      <c r="N13" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O13" s="24" t="s">
+      <c r="O13" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="P13" s="24" t="s">
+      <c r="P13" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q13" s="45" t="s">
+      <c r="Q13" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="R13" s="21">
+      <c r="R13" s="20">
         <v>201482</v>
       </c>
     </row>
@@ -8796,19 +8759,19 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AD889"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G13"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="4" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" style="2" customWidth="1"/>
@@ -8835,10 +8798,10 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -8853,7 +8816,7 @@
       <c r="K1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="34" t="s">
         <v>70</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -8880,43 +8843,42 @@
       <c r="AD1" s="2"/>
     </row>
     <row r="2" spans="1:30" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="29">
+      <c r="A2" s="28">
         <v>6545928</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="22" t="str">
-        <f>CONCATENATE(F2,B2,"Sp")</f>
-        <v>ScheduleEx6545928Sp</v>
-      </c>
-      <c r="H2" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="24">
         <v>1</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M2" s="22" t="s">
+      <c r="L2" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="22">
+      <c r="N2" s="21">
         <v>201480</v>
       </c>
     </row>
@@ -8925,37 +8887,36 @@
         <v>6546535</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="22" t="str">
-        <f t="shared" ref="G3:G13" si="0">CONCATENATE(F3,B3,"Sp")</f>
-        <v>Schedule6546535Sp</v>
-      </c>
-      <c r="H3" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="24">
         <v>1</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M3" s="22" t="s">
+      <c r="L3" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="22">
+      <c r="N3" s="21">
         <v>201480</v>
       </c>
     </row>
@@ -8964,37 +8925,36 @@
         <v>6596614</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Schedule6596614Sp</v>
-      </c>
-      <c r="H4" s="34" t="s">
+      <c r="F4" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="24">
         <v>1</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M4" s="22" t="s">
+      <c r="L4" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N4" s="22">
+      <c r="N4" s="21">
         <v>201480</v>
       </c>
     </row>
@@ -9003,232 +8963,226 @@
         <v>6596618</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Schedule6596618Sp</v>
-      </c>
-      <c r="H5" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="24">
         <v>1</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M5" s="22" t="s">
+      <c r="L5" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N5" s="22">
+      <c r="N5" s="21">
         <v>201480</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A6" s="29">
+      <c r="A6" s="28">
         <v>6596772</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="G6" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>ScheduleEx6596772Sp</v>
-      </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="24">
         <v>1</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M6" s="22" t="s">
+      <c r="L6" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N6" s="22">
+      <c r="N6" s="21">
         <v>201481</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A7" s="28">
+      <c r="A7" s="27">
         <v>6596919</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Schedule6596919Sp</v>
-      </c>
-      <c r="H7" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="24">
         <v>1</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M7" s="22" t="s">
+      <c r="L7" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N7" s="22">
+      <c r="N7" s="21">
         <v>201481</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A8" s="28">
+      <c r="A8" s="27">
         <v>6598612</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Schedule6598612Sp</v>
-      </c>
-      <c r="H8" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="24">
         <v>1</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M8" s="22" t="s">
+      <c r="L8" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N8" s="22">
+      <c r="N8" s="21">
         <v>201481</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A9" s="28">
+      <c r="A9" s="27">
         <v>6598662</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Schedule6598662Sp</v>
-      </c>
-      <c r="H9" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="24">
         <v>1</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M9" s="22" t="s">
+      <c r="L9" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N9" s="22">
+      <c r="N9" s="21">
         <v>201481</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A10" s="29">
+      <c r="A10" s="28">
         <v>6597034</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>ScheduleEx6597034Sp</v>
-      </c>
-      <c r="H10" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="24">
         <v>1</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M10" s="22" t="s">
+      <c r="L10" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N10" s="22">
+      <c r="N10" s="21">
         <v>201482</v>
       </c>
     </row>
@@ -9237,37 +9191,36 @@
         <v>6598609</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="G11" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Schedule6598609Sp</v>
-      </c>
-      <c r="H11" s="34" t="s">
+      <c r="G11" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="24">
         <v>1</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="26" t="s">
+      <c r="K11" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L11" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M11" s="22" t="s">
+      <c r="L11" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="21">
         <v>201482</v>
       </c>
     </row>
@@ -9276,37 +9229,36 @@
         <v>6598809</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Schedule6598809Sp</v>
-      </c>
-      <c r="H12" s="34" t="s">
+      <c r="G12" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="24">
         <v>1</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M12" s="22" t="s">
+      <c r="L12" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N12" s="22">
+      <c r="N12" s="21">
         <v>201482</v>
       </c>
     </row>
@@ -9315,37 +9267,36 @@
         <v>6598923</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Schedule6598923Sp</v>
-      </c>
-      <c r="H13" s="34" t="s">
+      <c r="G13" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="24">
         <v>1</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K13" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M13" s="22" t="s">
+      <c r="L13" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="21">
         <v>201482</v>
       </c>
     </row>
@@ -10236,8 +10187,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AB895"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -10260,58 +10211,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="M1" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="43" t="s">
+      <c r="N1" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="42" t="s">
+      <c r="O1" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="P1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="44" t="s">
+      <c r="Q1" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="R1" s="44" t="s">
+      <c r="R1" s="43" t="s">
         <v>64</v>
       </c>
       <c r="S1" s="2"/>
@@ -10326,52 +10277,52 @@
       <c r="AB1" s="2"/>
     </row>
     <row r="2" spans="1:28" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="29">
+      <c r="A2" s="28">
         <v>6545928</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="36" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="37" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O2" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P2" s="34" t="s">
+      <c r="O2" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="34" t="s">
+      <c r="Q2" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R2" s="38">
+      <c r="R2" s="37">
         <v>201480</v>
       </c>
     </row>
@@ -10379,47 +10330,47 @@
       <c r="A3" s="15">
         <v>6546535</v>
       </c>
-      <c r="D3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" s="36" t="s">
+      <c r="D3" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="K3" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="38"/>
-      <c r="M3" s="37" t="s">
+      <c r="L3" s="37"/>
+      <c r="M3" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P3" s="34" t="s">
+      <c r="O3" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="Q3" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R3" s="38">
+      <c r="R3" s="37">
         <v>201480</v>
       </c>
     </row>
@@ -10427,46 +10378,46 @@
       <c r="A4" s="15">
         <v>6596614</v>
       </c>
-      <c r="D4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="36" t="s">
+      <c r="D4" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="34" t="s">
+      <c r="J4" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="34" t="s">
+      <c r="K4" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="N4" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P4" s="34" t="s">
+      <c r="O4" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q4" s="34" t="s">
+      <c r="Q4" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="38">
+      <c r="R4" s="37">
         <v>201480</v>
       </c>
     </row>
@@ -10474,281 +10425,281 @@
       <c r="A5" s="15">
         <v>6596618</v>
       </c>
-      <c r="D5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="36" t="s">
+      <c r="D5" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="37" t="s">
+      <c r="M5" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N5" s="37" t="s">
+      <c r="N5" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O5" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P5" s="34" t="s">
+      <c r="O5" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q5" s="34" t="s">
+      <c r="Q5" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R5" s="38">
+      <c r="R5" s="37">
         <v>201480</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A6" s="29">
+      <c r="A6" s="28">
         <v>6596772</v>
       </c>
-      <c r="D6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" s="36" t="s">
+      <c r="D6" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="34" t="s">
+      <c r="K6" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="37" t="s">
+      <c r="M6" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P6" s="34" t="s">
+      <c r="O6" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" s="34" t="s">
+      <c r="Q6" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R6" s="38">
+      <c r="R6" s="37">
         <v>201481</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A7" s="28">
+      <c r="A7" s="27">
         <v>6596919</v>
       </c>
-      <c r="D7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="36" t="s">
+      <c r="D7" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="37" t="s">
+      <c r="M7" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="N7" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O7" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P7" s="34" t="s">
+      <c r="O7" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q7" s="34" t="s">
+      <c r="Q7" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R7" s="38">
+      <c r="R7" s="37">
         <v>201481</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A8" s="28">
+      <c r="A8" s="27">
         <v>6598612</v>
       </c>
-      <c r="D8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" s="36" t="s">
+      <c r="D8" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="37" t="s">
+      <c r="N8" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O8" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P8" s="34" t="s">
+      <c r="O8" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q8" s="34" t="s">
+      <c r="Q8" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R8" s="38">
+      <c r="R8" s="37">
         <v>201481</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A9" s="28">
+      <c r="A9" s="27">
         <v>6598662</v>
       </c>
-      <c r="D9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="36" t="s">
+      <c r="D9" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="J9" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="34" t="s">
+      <c r="K9" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="M9" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O9" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P9" s="34" t="s">
+      <c r="O9" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P9" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="Q9" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R9" s="38">
+      <c r="R9" s="37">
         <v>201481</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A10" s="29">
+      <c r="A10" s="28">
         <v>6597034</v>
       </c>
-      <c r="D10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="36" t="s">
+      <c r="D10" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="34" t="s">
+      <c r="J10" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="34" t="s">
+      <c r="K10" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="37" t="s">
+      <c r="M10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="37" t="s">
+      <c r="N10" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O10" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P10" s="34" t="s">
+      <c r="O10" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P10" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q10" s="34" t="s">
+      <c r="Q10" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R10" s="38">
+      <c r="R10" s="37">
         <v>201482</v>
       </c>
     </row>
@@ -10756,46 +10707,46 @@
       <c r="A11" s="15">
         <v>6598609</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E11" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" s="36" t="s">
+      <c r="E11" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="K11" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M11" s="37" t="s">
+      <c r="M11" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="37" t="s">
+      <c r="N11" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O11" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P11" s="34" t="s">
+      <c r="O11" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P11" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q11" s="34" t="s">
+      <c r="Q11" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R11" s="38">
+      <c r="R11" s="37">
         <v>201482</v>
       </c>
     </row>
@@ -10803,46 +10754,46 @@
       <c r="A12" s="15">
         <v>6598809</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E12" t="s">
-        <v>103</v>
-      </c>
-      <c r="F12" s="36" t="s">
+      <c r="E12" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="34" t="s">
+      <c r="J12" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="34" t="s">
+      <c r="K12" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M12" s="37" t="s">
+      <c r="M12" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N12" s="37" t="s">
+      <c r="N12" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O12" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P12" s="34" t="s">
+      <c r="O12" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P12" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q12" s="34" t="s">
+      <c r="Q12" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R12" s="38">
+      <c r="R12" s="37">
         <v>201482</v>
       </c>
     </row>
@@ -10850,46 +10801,46 @@
       <c r="A13" s="15">
         <v>6598923</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E13" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="36" t="s">
+      <c r="E13" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G13" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="J13" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="34" t="s">
+      <c r="K13" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M13" s="37" t="s">
+      <c r="M13" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="N13" s="37" t="s">
+      <c r="N13" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O13" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P13" s="34" t="s">
+      <c r="O13" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="P13" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="Q13" s="34" t="s">
+      <c r="Q13" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="R13" s="38">
+      <c r="R13" s="37">
         <v>201482</v>
       </c>
     </row>

</xml_diff>